<commit_message>
Updated Document Projekt ICT-BZ Updated Zeitplan
</commit_message>
<xml_diff>
--- a/Documents/Zeitplanung.xlsx
+++ b/Documents/Zeitplanung.xlsx
@@ -300,12 +300,6 @@
     <t>Anforderung #03 (Pflanzen-Daten per SMS)</t>
   </si>
   <si>
-    <t>Anforderung #04 (Pflanzen-Daten im Blog-Format (Website))</t>
-  </si>
-  <si>
-    <t>Anforderung #05 (Pflanzen-Daten auf Website)</t>
-  </si>
-  <si>
     <t>Anforderung #06 (Website: Pflanze Über mich Seite)</t>
   </si>
   <si>
@@ -324,16 +318,22 @@
     <t>Anforderung #11 (Admin: Twitter-Account)</t>
   </si>
   <si>
-    <t>Anforderung #12 (Admin: Twitter-Account)</t>
-  </si>
-  <si>
     <t>Projektende</t>
   </si>
   <si>
     <t>Geplant</t>
   </si>
   <si>
-    <t>§1.5</t>
+    <t>Anforderung #04 (Pflalnze: Webseite)</t>
+  </si>
+  <si>
+    <t>Anforderung #05 (Pflanzen-Daten auf Website im Blog-Format)</t>
+  </si>
+  <si>
+    <t>Anforderung #12 (Admin: Tweets löschen)</t>
+  </si>
+  <si>
+    <t>Geschaft</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,6 +547,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="81">
     <border>
@@ -1560,7 +1572,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1879,6 +1891,261 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="73" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="74" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="55" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="56" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="56" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="75" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="76" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="53" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="53" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="75" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="74" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1923,246 +2190,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="73" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="74" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="55" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="56" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="56" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="75" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="76" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="53" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="53" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="75" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="74" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
@@ -2175,10 +2202,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
       <color rgb="FF00FF00"/>
       <color rgb="FFFF9999"/>
       <color rgb="FFCCC0DA"/>
-      <color rgb="FFFFFF66"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2222,7 +2249,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2384,13 +2410,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>6.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2399,13 +2425,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2444,13 +2470,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2470,11 +2496,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="309381064"/>
-        <c:axId val="309381848"/>
+        <c:axId val="321404104"/>
+        <c:axId val="321397048"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="309381064"/>
+        <c:axId val="321404104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2484,14 +2510,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309381848"/>
+        <c:crossAx val="321397048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="309381848"/>
+        <c:axId val="321397048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2502,14 +2528,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309381064"/>
+        <c:crossAx val="321404104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2593,7 +2618,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
@@ -2667,13 +2692,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>13.2</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2702,11 +2727,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="309383808"/>
-        <c:axId val="309379888"/>
+        <c:axId val="321397832"/>
+        <c:axId val="321398224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="309383808"/>
+        <c:axId val="321397832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2716,7 +2741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309379888"/>
+        <c:crossAx val="321398224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2724,7 +2749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309379888"/>
+        <c:axId val="321398224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,14 +2760,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309383808"/>
+        <c:crossAx val="321397832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3177,8 +3201,8 @@
   </sheetPr>
   <dimension ref="A1:AS44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3193,46 +3217,46 @@
     <col min="11" max="30" width="3.25" style="5" customWidth="1"/>
     <col min="31" max="35" width="3.25" style="4" customWidth="1"/>
     <col min="36" max="40" width="3.08203125" style="4" customWidth="1"/>
-    <col min="41" max="42" width="2.9140625" style="5" customWidth="1"/>
-    <col min="43" max="43" width="2.6640625" style="5" customWidth="1"/>
+    <col min="41" max="42" width="2.83203125" style="5" customWidth="1"/>
+    <col min="43" max="43" width="2.58203125" style="5" customWidth="1"/>
     <col min="44" max="44" width="4" style="5" customWidth="1"/>
     <col min="45" max="45" width="3.25" style="5" customWidth="1"/>
     <col min="46" max="16384" width="12.5" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="194" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
-      <c r="U1" s="109"/>
-      <c r="V1" s="109"/>
-      <c r="W1" s="109"/>
-      <c r="X1" s="109"/>
-      <c r="Y1" s="109"/>
-      <c r="Z1" s="109"/>
-      <c r="AA1" s="109"/>
-      <c r="AB1" s="109"/>
-      <c r="AC1" s="109"/>
-      <c r="AD1" s="109"/>
+      <c r="B1" s="194"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="194"/>
+      <c r="H1" s="194"/>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
+      <c r="L1" s="194"/>
+      <c r="M1" s="194"/>
+      <c r="N1" s="194"/>
+      <c r="O1" s="194"/>
+      <c r="P1" s="194"/>
+      <c r="Q1" s="194"/>
+      <c r="R1" s="194"/>
+      <c r="S1" s="194"/>
+      <c r="T1" s="194"/>
+      <c r="U1" s="194"/>
+      <c r="V1" s="194"/>
+      <c r="W1" s="194"/>
+      <c r="X1" s="194"/>
+      <c r="Y1" s="194"/>
+      <c r="Z1" s="194"/>
+      <c r="AA1" s="194"/>
+      <c r="AB1" s="194"/>
+      <c r="AC1" s="194"/>
+      <c r="AD1" s="194"/>
     </row>
     <row r="2" spans="1:45" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -3251,65 +3275,65 @@
     <row r="3" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="52"/>
       <c r="B3" s="56"/>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="196" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="111"/>
+      <c r="D3" s="196"/>
       <c r="E3" s="16"/>
       <c r="F3" s="17"/>
       <c r="G3" s="19"/>
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="111" t="s">
+      <c r="K3" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
-      <c r="N3" s="111"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="110" t="s">
+      <c r="L3" s="196"/>
+      <c r="M3" s="196"/>
+      <c r="N3" s="196"/>
+      <c r="O3" s="197"/>
+      <c r="P3" s="195" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="111"/>
-      <c r="R3" s="111"/>
-      <c r="S3" s="111"/>
-      <c r="T3" s="111"/>
-      <c r="U3" s="110" t="s">
+      <c r="Q3" s="196"/>
+      <c r="R3" s="196"/>
+      <c r="S3" s="196"/>
+      <c r="T3" s="196"/>
+      <c r="U3" s="195" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="111"/>
-      <c r="W3" s="111"/>
-      <c r="X3" s="111"/>
-      <c r="Y3" s="111"/>
-      <c r="Z3" s="110" t="s">
+      <c r="V3" s="196"/>
+      <c r="W3" s="196"/>
+      <c r="X3" s="196"/>
+      <c r="Y3" s="196"/>
+      <c r="Z3" s="195" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="111"/>
-      <c r="AB3" s="111"/>
-      <c r="AC3" s="111"/>
-      <c r="AD3" s="111"/>
-      <c r="AE3" s="110" t="s">
+      <c r="AA3" s="196"/>
+      <c r="AB3" s="196"/>
+      <c r="AC3" s="196"/>
+      <c r="AD3" s="196"/>
+      <c r="AE3" s="195" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" s="111"/>
-      <c r="AG3" s="111"/>
-      <c r="AH3" s="111"/>
-      <c r="AI3" s="111"/>
-      <c r="AJ3" s="110" t="s">
+      <c r="AF3" s="196"/>
+      <c r="AG3" s="196"/>
+      <c r="AH3" s="196"/>
+      <c r="AI3" s="196"/>
+      <c r="AJ3" s="195" t="s">
         <v>35</v>
       </c>
-      <c r="AK3" s="111"/>
-      <c r="AL3" s="111"/>
-      <c r="AM3" s="111"/>
-      <c r="AN3" s="113"/>
-      <c r="AO3" s="110" t="s">
+      <c r="AK3" s="196"/>
+      <c r="AL3" s="196"/>
+      <c r="AM3" s="196"/>
+      <c r="AN3" s="198"/>
+      <c r="AO3" s="195" t="s">
         <v>35</v>
       </c>
-      <c r="AP3" s="111"/>
-      <c r="AQ3" s="111"/>
-      <c r="AR3" s="111"/>
-      <c r="AS3" s="113"/>
+      <c r="AP3" s="196"/>
+      <c r="AQ3" s="196"/>
+      <c r="AR3" s="196"/>
+      <c r="AS3" s="198"/>
     </row>
     <row r="4" spans="1:45" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="87" t="s">
@@ -3488,11 +3512,11 @@
       </c>
       <c r="C5" s="75">
         <f>SUM(C6:C10)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D5" s="76">
         <f>SUM(D6:D10)</f>
-        <v>13.2</v>
+        <v>8.9</v>
       </c>
       <c r="E5" s="77"/>
       <c r="F5" s="78"/>
@@ -3558,43 +3582,43 @@
       <c r="H6" s="34"/>
       <c r="I6" s="35"/>
       <c r="J6" s="66"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="127">
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="111">
         <v>2</v>
       </c>
-      <c r="N6" s="128"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="130"/>
-      <c r="Q6" s="131"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="132"/>
-      <c r="T6" s="133"/>
-      <c r="U6" s="130"/>
-      <c r="V6" s="131"/>
-      <c r="W6" s="127"/>
-      <c r="X6" s="132"/>
-      <c r="Y6" s="133"/>
-      <c r="Z6" s="134"/>
-      <c r="AA6" s="135"/>
-      <c r="AB6" s="128"/>
-      <c r="AC6" s="135"/>
-      <c r="AD6" s="136"/>
-      <c r="AE6" s="134"/>
-      <c r="AF6" s="135"/>
-      <c r="AG6" s="128"/>
-      <c r="AH6" s="135"/>
-      <c r="AI6" s="136"/>
-      <c r="AJ6" s="137"/>
-      <c r="AK6" s="131"/>
-      <c r="AL6" s="132"/>
-      <c r="AM6" s="132"/>
-      <c r="AN6" s="138"/>
-      <c r="AO6" s="137"/>
-      <c r="AP6" s="131"/>
-      <c r="AQ6" s="132"/>
-      <c r="AR6" s="132"/>
-      <c r="AS6" s="138"/>
+      <c r="N6" s="112"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="114"/>
+      <c r="Q6" s="115"/>
+      <c r="R6" s="111"/>
+      <c r="S6" s="116"/>
+      <c r="T6" s="117"/>
+      <c r="U6" s="114"/>
+      <c r="V6" s="115"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="116"/>
+      <c r="Y6" s="117"/>
+      <c r="Z6" s="118"/>
+      <c r="AA6" s="119"/>
+      <c r="AB6" s="112"/>
+      <c r="AC6" s="119"/>
+      <c r="AD6" s="120"/>
+      <c r="AE6" s="118"/>
+      <c r="AF6" s="119"/>
+      <c r="AG6" s="112"/>
+      <c r="AH6" s="119"/>
+      <c r="AI6" s="120"/>
+      <c r="AJ6" s="121"/>
+      <c r="AK6" s="115"/>
+      <c r="AL6" s="116"/>
+      <c r="AM6" s="116"/>
+      <c r="AN6" s="122"/>
+      <c r="AO6" s="121"/>
+      <c r="AP6" s="115"/>
+      <c r="AQ6" s="116"/>
+      <c r="AR6" s="116"/>
+      <c r="AS6" s="122"/>
     </row>
     <row r="7" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53">
@@ -3618,43 +3642,43 @@
       <c r="H7" s="34"/>
       <c r="I7" s="35"/>
       <c r="J7" s="67"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="140"/>
-      <c r="O7" s="129"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="127">
+      <c r="K7" s="109"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="123"/>
+      <c r="N7" s="124"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="180">
         <v>6</v>
       </c>
-      <c r="S7" s="143"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="141"/>
-      <c r="V7" s="142"/>
-      <c r="W7" s="127"/>
-      <c r="X7" s="143"/>
-      <c r="Y7" s="144"/>
-      <c r="Z7" s="145"/>
-      <c r="AA7" s="146"/>
-      <c r="AB7" s="128"/>
-      <c r="AC7" s="146"/>
-      <c r="AD7" s="147"/>
-      <c r="AE7" s="145"/>
-      <c r="AF7" s="146"/>
-      <c r="AG7" s="128"/>
-      <c r="AH7" s="146"/>
-      <c r="AI7" s="147"/>
-      <c r="AJ7" s="148"/>
-      <c r="AK7" s="142"/>
-      <c r="AL7" s="143"/>
-      <c r="AM7" s="143"/>
-      <c r="AN7" s="149"/>
-      <c r="AO7" s="148"/>
-      <c r="AP7" s="142"/>
-      <c r="AQ7" s="143"/>
-      <c r="AR7" s="143"/>
-      <c r="AS7" s="149"/>
+      <c r="S7" s="127"/>
+      <c r="T7" s="128"/>
+      <c r="U7" s="125"/>
+      <c r="V7" s="126"/>
+      <c r="W7" s="111"/>
+      <c r="X7" s="127"/>
+      <c r="Y7" s="128"/>
+      <c r="Z7" s="129"/>
+      <c r="AA7" s="130"/>
+      <c r="AB7" s="112"/>
+      <c r="AC7" s="130"/>
+      <c r="AD7" s="131"/>
+      <c r="AE7" s="129"/>
+      <c r="AF7" s="130"/>
+      <c r="AG7" s="112"/>
+      <c r="AH7" s="130"/>
+      <c r="AI7" s="131"/>
+      <c r="AJ7" s="132"/>
+      <c r="AK7" s="126"/>
+      <c r="AL7" s="127"/>
+      <c r="AM7" s="127"/>
+      <c r="AN7" s="133"/>
+      <c r="AO7" s="132"/>
+      <c r="AP7" s="126"/>
+      <c r="AQ7" s="127"/>
+      <c r="AR7" s="127"/>
+      <c r="AS7" s="133"/>
     </row>
     <row r="8" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="53">
@@ -3664,11 +3688,11 @@
         <v>37</v>
       </c>
       <c r="C8" s="37">
-        <v>2</v>
-      </c>
-      <c r="D8" s="33">
+        <v>8</v>
+      </c>
+      <c r="D8" s="33" t="str">
         <f>IF(SUM(K8:AS8)=0," ",SUM(K8:AS8))</f>
-        <v>4.5</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E8" s="36">
         <v>1</v>
@@ -3678,49 +3702,41 @@
       <c r="H8" s="34"/>
       <c r="I8" s="35"/>
       <c r="J8" s="67"/>
-      <c r="K8" s="125"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="139"/>
-      <c r="N8" s="140"/>
-      <c r="O8" s="129"/>
-      <c r="P8" s="141"/>
-      <c r="Q8" s="142"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="143"/>
-      <c r="T8" s="196">
-        <v>1.5</v>
-      </c>
-      <c r="U8" s="141"/>
-      <c r="V8" s="142"/>
-      <c r="W8" s="127"/>
-      <c r="X8" s="143"/>
-      <c r="Y8" s="196">
-        <v>1.5</v>
-      </c>
-      <c r="Z8" s="145"/>
-      <c r="AA8" s="146"/>
-      <c r="AB8" s="128"/>
-      <c r="AC8" s="146"/>
-      <c r="AD8" s="147"/>
-      <c r="AE8" s="145"/>
-      <c r="AF8" s="146"/>
-      <c r="AG8" s="128"/>
-      <c r="AH8" s="146"/>
-      <c r="AI8" s="147"/>
-      <c r="AJ8" s="148"/>
-      <c r="AK8" s="142"/>
-      <c r="AL8" s="143"/>
-      <c r="AM8" s="150"/>
-      <c r="AN8" s="203">
-        <v>1.5</v>
-      </c>
-      <c r="AO8" s="148"/>
-      <c r="AP8" s="142"/>
-      <c r="AQ8" s="143"/>
-      <c r="AR8" s="150"/>
-      <c r="AS8" s="203" t="s">
-        <v>57</v>
-      </c>
+      <c r="K8" s="109"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="123"/>
+      <c r="N8" s="124"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="127"/>
+      <c r="T8" s="188"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="126"/>
+      <c r="W8" s="111"/>
+      <c r="X8" s="127"/>
+      <c r="Y8" s="192"/>
+      <c r="Z8" s="129"/>
+      <c r="AA8" s="130"/>
+      <c r="AB8" s="112"/>
+      <c r="AC8" s="130"/>
+      <c r="AD8" s="131"/>
+      <c r="AE8" s="129"/>
+      <c r="AF8" s="130"/>
+      <c r="AG8" s="112"/>
+      <c r="AH8" s="130"/>
+      <c r="AI8" s="131"/>
+      <c r="AJ8" s="132"/>
+      <c r="AK8" s="126"/>
+      <c r="AL8" s="127"/>
+      <c r="AM8" s="134"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="132"/>
+      <c r="AP8" s="126"/>
+      <c r="AQ8" s="127"/>
+      <c r="AR8" s="134"/>
+      <c r="AS8" s="187"/>
     </row>
     <row r="9" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="53">
@@ -3734,7 +3750,7 @@
       </c>
       <c r="D9" s="33">
         <f>IF(SUM(K9:AS9)=0," ",SUM(K9:AS9))</f>
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E9" s="36">
         <v>1</v>
@@ -3744,45 +3760,45 @@
       <c r="H9" s="34"/>
       <c r="I9" s="35"/>
       <c r="J9" s="67"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="126"/>
-      <c r="M9" s="139"/>
-      <c r="N9" s="140"/>
-      <c r="O9" s="129"/>
-      <c r="P9" s="141"/>
-      <c r="Q9" s="142"/>
-      <c r="R9" s="127">
+      <c r="K9" s="109"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="124"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="126"/>
+      <c r="R9" s="180">
         <v>0.4</v>
       </c>
-      <c r="S9" s="195">
-        <v>0.3</v>
-      </c>
-      <c r="T9" s="144"/>
-      <c r="U9" s="141"/>
-      <c r="V9" s="142"/>
-      <c r="W9" s="127"/>
-      <c r="X9" s="143"/>
-      <c r="Y9" s="144"/>
-      <c r="Z9" s="145"/>
-      <c r="AA9" s="146"/>
-      <c r="AB9" s="128"/>
-      <c r="AC9" s="146"/>
-      <c r="AD9" s="147"/>
-      <c r="AE9" s="145"/>
-      <c r="AF9" s="146"/>
-      <c r="AG9" s="128"/>
-      <c r="AH9" s="146"/>
-      <c r="AI9" s="147"/>
-      <c r="AJ9" s="141"/>
-      <c r="AK9" s="142"/>
-      <c r="AL9" s="143"/>
-      <c r="AM9" s="150"/>
-      <c r="AN9" s="151"/>
-      <c r="AO9" s="141"/>
-      <c r="AP9" s="142"/>
-      <c r="AQ9" s="143"/>
-      <c r="AR9" s="150"/>
-      <c r="AS9" s="151"/>
+      <c r="S9" s="179">
+        <v>0.5</v>
+      </c>
+      <c r="T9" s="128"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="126"/>
+      <c r="W9" s="191"/>
+      <c r="X9" s="127"/>
+      <c r="Y9" s="192"/>
+      <c r="Z9" s="129"/>
+      <c r="AA9" s="130"/>
+      <c r="AB9" s="112"/>
+      <c r="AC9" s="130"/>
+      <c r="AD9" s="131"/>
+      <c r="AE9" s="129"/>
+      <c r="AF9" s="130"/>
+      <c r="AG9" s="112"/>
+      <c r="AH9" s="130"/>
+      <c r="AI9" s="131"/>
+      <c r="AJ9" s="125"/>
+      <c r="AK9" s="126"/>
+      <c r="AL9" s="127"/>
+      <c r="AM9" s="134"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="125"/>
+      <c r="AP9" s="126"/>
+      <c r="AQ9" s="181"/>
+      <c r="AR9" s="134"/>
+      <c r="AS9" s="135"/>
     </row>
     <row r="10" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="53">
@@ -3806,41 +3822,41 @@
       <c r="H10" s="39"/>
       <c r="I10" s="35"/>
       <c r="J10" s="67"/>
-      <c r="K10" s="125"/>
-      <c r="L10" s="126"/>
-      <c r="M10" s="152"/>
-      <c r="N10" s="153"/>
-      <c r="O10" s="154"/>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="156"/>
-      <c r="R10" s="157"/>
-      <c r="S10" s="158"/>
-      <c r="T10" s="159"/>
-      <c r="U10" s="155"/>
-      <c r="V10" s="156"/>
-      <c r="W10" s="157"/>
-      <c r="X10" s="158"/>
-      <c r="Y10" s="159"/>
-      <c r="Z10" s="160"/>
-      <c r="AA10" s="161"/>
-      <c r="AB10" s="162"/>
-      <c r="AC10" s="161"/>
-      <c r="AD10" s="163"/>
-      <c r="AE10" s="160"/>
-      <c r="AF10" s="161"/>
-      <c r="AG10" s="162"/>
-      <c r="AH10" s="161"/>
-      <c r="AI10" s="163"/>
-      <c r="AJ10" s="164"/>
-      <c r="AK10" s="156"/>
-      <c r="AL10" s="158"/>
-      <c r="AM10" s="165"/>
-      <c r="AN10" s="151"/>
-      <c r="AO10" s="164"/>
-      <c r="AP10" s="156"/>
-      <c r="AQ10" s="158"/>
-      <c r="AR10" s="165"/>
-      <c r="AS10" s="151"/>
+      <c r="K10" s="109"/>
+      <c r="L10" s="110"/>
+      <c r="M10" s="136"/>
+      <c r="N10" s="137"/>
+      <c r="O10" s="138"/>
+      <c r="P10" s="139"/>
+      <c r="Q10" s="140"/>
+      <c r="R10" s="141"/>
+      <c r="S10" s="142"/>
+      <c r="T10" s="143"/>
+      <c r="U10" s="139"/>
+      <c r="V10" s="140"/>
+      <c r="W10" s="141"/>
+      <c r="X10" s="142"/>
+      <c r="Y10" s="143"/>
+      <c r="Z10" s="144"/>
+      <c r="AA10" s="145"/>
+      <c r="AB10" s="146"/>
+      <c r="AC10" s="145"/>
+      <c r="AD10" s="147"/>
+      <c r="AE10" s="144"/>
+      <c r="AF10" s="145"/>
+      <c r="AG10" s="146"/>
+      <c r="AH10" s="145"/>
+      <c r="AI10" s="147"/>
+      <c r="AJ10" s="148"/>
+      <c r="AK10" s="140"/>
+      <c r="AL10" s="142"/>
+      <c r="AM10" s="149"/>
+      <c r="AN10" s="135"/>
+      <c r="AO10" s="148"/>
+      <c r="AP10" s="140"/>
+      <c r="AQ10" s="142"/>
+      <c r="AR10" s="149"/>
+      <c r="AS10" s="135"/>
     </row>
     <row r="11" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="72">
@@ -3863,41 +3879,41 @@
       <c r="H11" s="79"/>
       <c r="I11" s="80"/>
       <c r="J11" s="81"/>
-      <c r="K11" s="166"/>
-      <c r="L11" s="167"/>
-      <c r="M11" s="168"/>
-      <c r="N11" s="169"/>
-      <c r="O11" s="170"/>
-      <c r="P11" s="171"/>
-      <c r="Q11" s="168"/>
-      <c r="R11" s="169"/>
-      <c r="S11" s="167"/>
-      <c r="T11" s="172"/>
-      <c r="U11" s="171"/>
-      <c r="V11" s="168"/>
-      <c r="W11" s="169"/>
-      <c r="X11" s="167"/>
-      <c r="Y11" s="172"/>
-      <c r="Z11" s="171"/>
-      <c r="AA11" s="168"/>
-      <c r="AB11" s="169"/>
-      <c r="AC11" s="167"/>
-      <c r="AD11" s="172"/>
-      <c r="AE11" s="171"/>
-      <c r="AF11" s="168"/>
-      <c r="AG11" s="169"/>
-      <c r="AH11" s="167"/>
-      <c r="AI11" s="172"/>
-      <c r="AJ11" s="171"/>
-      <c r="AK11" s="168"/>
-      <c r="AL11" s="168"/>
-      <c r="AM11" s="169"/>
-      <c r="AN11" s="173"/>
-      <c r="AO11" s="171"/>
-      <c r="AP11" s="168"/>
-      <c r="AQ11" s="168"/>
-      <c r="AR11" s="169"/>
-      <c r="AS11" s="173"/>
+      <c r="K11" s="150"/>
+      <c r="L11" s="151"/>
+      <c r="M11" s="152"/>
+      <c r="N11" s="153"/>
+      <c r="O11" s="154"/>
+      <c r="P11" s="155"/>
+      <c r="Q11" s="152"/>
+      <c r="R11" s="153"/>
+      <c r="S11" s="151"/>
+      <c r="T11" s="156"/>
+      <c r="U11" s="155"/>
+      <c r="V11" s="152"/>
+      <c r="W11" s="153"/>
+      <c r="X11" s="151"/>
+      <c r="Y11" s="156"/>
+      <c r="Z11" s="155"/>
+      <c r="AA11" s="152"/>
+      <c r="AB11" s="153"/>
+      <c r="AC11" s="151"/>
+      <c r="AD11" s="156"/>
+      <c r="AE11" s="155"/>
+      <c r="AF11" s="152"/>
+      <c r="AG11" s="153"/>
+      <c r="AH11" s="151"/>
+      <c r="AI11" s="156"/>
+      <c r="AJ11" s="155"/>
+      <c r="AK11" s="152"/>
+      <c r="AL11" s="152"/>
+      <c r="AM11" s="153"/>
+      <c r="AN11" s="157"/>
+      <c r="AO11" s="155"/>
+      <c r="AP11" s="152"/>
+      <c r="AQ11" s="152"/>
+      <c r="AR11" s="153"/>
+      <c r="AS11" s="157"/>
     </row>
     <row r="12" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="54">
@@ -3921,45 +3937,45 @@
       <c r="H12" s="34"/>
       <c r="I12" s="35"/>
       <c r="J12" s="67"/>
-      <c r="K12" s="174"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="139">
+      <c r="K12" s="158"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="123">
         <v>5</v>
       </c>
-      <c r="N12" s="128"/>
-      <c r="O12" s="129"/>
-      <c r="P12" s="130"/>
-      <c r="Q12" s="131"/>
-      <c r="R12" s="127">
+      <c r="N12" s="112"/>
+      <c r="O12" s="113"/>
+      <c r="P12" s="114"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="180">
         <v>0.5</v>
       </c>
-      <c r="S12" s="132"/>
-      <c r="T12" s="132"/>
-      <c r="U12" s="130"/>
-      <c r="V12" s="131"/>
-      <c r="W12" s="127"/>
-      <c r="X12" s="132"/>
-      <c r="Y12" s="132"/>
-      <c r="Z12" s="134"/>
-      <c r="AA12" s="135"/>
-      <c r="AB12" s="128"/>
-      <c r="AC12" s="135"/>
-      <c r="AD12" s="135"/>
-      <c r="AE12" s="134"/>
-      <c r="AF12" s="135"/>
-      <c r="AG12" s="128"/>
-      <c r="AH12" s="135"/>
-      <c r="AI12" s="135"/>
-      <c r="AJ12" s="137"/>
-      <c r="AK12" s="131"/>
-      <c r="AL12" s="132"/>
-      <c r="AM12" s="175"/>
-      <c r="AN12" s="176"/>
-      <c r="AO12" s="137"/>
-      <c r="AP12" s="131"/>
-      <c r="AQ12" s="132"/>
-      <c r="AR12" s="175"/>
-      <c r="AS12" s="176"/>
+      <c r="S12" s="116"/>
+      <c r="T12" s="116"/>
+      <c r="U12" s="114"/>
+      <c r="V12" s="115"/>
+      <c r="W12" s="111"/>
+      <c r="X12" s="116"/>
+      <c r="Y12" s="116"/>
+      <c r="Z12" s="118"/>
+      <c r="AA12" s="119"/>
+      <c r="AB12" s="112"/>
+      <c r="AC12" s="119"/>
+      <c r="AD12" s="119"/>
+      <c r="AE12" s="118"/>
+      <c r="AF12" s="119"/>
+      <c r="AG12" s="112"/>
+      <c r="AH12" s="119"/>
+      <c r="AI12" s="119"/>
+      <c r="AJ12" s="121"/>
+      <c r="AK12" s="115"/>
+      <c r="AL12" s="116"/>
+      <c r="AM12" s="159"/>
+      <c r="AN12" s="160"/>
+      <c r="AO12" s="121"/>
+      <c r="AP12" s="115"/>
+      <c r="AQ12" s="116"/>
+      <c r="AR12" s="159"/>
+      <c r="AS12" s="160"/>
     </row>
     <row r="13" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="54">
@@ -3974,41 +3990,41 @@
       <c r="H13" s="34"/>
       <c r="I13" s="35"/>
       <c r="J13" s="67"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="126"/>
-      <c r="M13" s="139"/>
-      <c r="N13" s="128"/>
-      <c r="O13" s="129"/>
-      <c r="P13" s="130"/>
-      <c r="Q13" s="131"/>
-      <c r="R13" s="127"/>
-      <c r="S13" s="132"/>
-      <c r="T13" s="132"/>
-      <c r="U13" s="130"/>
-      <c r="V13" s="131"/>
-      <c r="W13" s="127"/>
-      <c r="X13" s="132"/>
-      <c r="Y13" s="132"/>
-      <c r="Z13" s="134"/>
-      <c r="AA13" s="135"/>
-      <c r="AB13" s="128"/>
-      <c r="AC13" s="135"/>
-      <c r="AD13" s="135"/>
-      <c r="AE13" s="134"/>
-      <c r="AF13" s="135"/>
-      <c r="AG13" s="128"/>
-      <c r="AH13" s="135"/>
-      <c r="AI13" s="135"/>
-      <c r="AJ13" s="137"/>
-      <c r="AK13" s="131"/>
-      <c r="AL13" s="132"/>
-      <c r="AM13" s="175"/>
-      <c r="AN13" s="176"/>
-      <c r="AO13" s="137"/>
-      <c r="AP13" s="131"/>
-      <c r="AQ13" s="132"/>
-      <c r="AR13" s="175"/>
-      <c r="AS13" s="176"/>
+      <c r="K13" s="158"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="123"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="114"/>
+      <c r="Q13" s="115"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="116"/>
+      <c r="T13" s="116"/>
+      <c r="U13" s="114"/>
+      <c r="V13" s="115"/>
+      <c r="W13" s="111"/>
+      <c r="X13" s="116"/>
+      <c r="Y13" s="116"/>
+      <c r="Z13" s="118"/>
+      <c r="AA13" s="119"/>
+      <c r="AB13" s="112"/>
+      <c r="AC13" s="119"/>
+      <c r="AD13" s="119"/>
+      <c r="AE13" s="118"/>
+      <c r="AF13" s="119"/>
+      <c r="AG13" s="112"/>
+      <c r="AH13" s="119"/>
+      <c r="AI13" s="119"/>
+      <c r="AJ13" s="121"/>
+      <c r="AK13" s="115"/>
+      <c r="AL13" s="116"/>
+      <c r="AM13" s="159"/>
+      <c r="AN13" s="160"/>
+      <c r="AO13" s="121"/>
+      <c r="AP13" s="115"/>
+      <c r="AQ13" s="116"/>
+      <c r="AR13" s="159"/>
+      <c r="AS13" s="160"/>
     </row>
     <row r="14" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="54">
@@ -4023,41 +4039,41 @@
       <c r="H14" s="34"/>
       <c r="I14" s="35"/>
       <c r="J14" s="67"/>
-      <c r="K14" s="174"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="139"/>
-      <c r="N14" s="128"/>
-      <c r="O14" s="129"/>
-      <c r="P14" s="130"/>
-      <c r="Q14" s="131"/>
-      <c r="R14" s="127"/>
-      <c r="S14" s="132"/>
-      <c r="T14" s="132"/>
-      <c r="U14" s="130"/>
-      <c r="V14" s="131"/>
-      <c r="W14" s="127"/>
-      <c r="X14" s="132"/>
-      <c r="Y14" s="132"/>
-      <c r="Z14" s="134"/>
-      <c r="AA14" s="135"/>
-      <c r="AB14" s="128"/>
-      <c r="AC14" s="135"/>
-      <c r="AD14" s="135"/>
-      <c r="AE14" s="134"/>
-      <c r="AF14" s="135"/>
-      <c r="AG14" s="128"/>
-      <c r="AH14" s="135"/>
-      <c r="AI14" s="135"/>
-      <c r="AJ14" s="137"/>
-      <c r="AK14" s="131"/>
-      <c r="AL14" s="132"/>
-      <c r="AM14" s="175"/>
-      <c r="AN14" s="176"/>
-      <c r="AO14" s="137"/>
-      <c r="AP14" s="131"/>
-      <c r="AQ14" s="132"/>
-      <c r="AR14" s="175"/>
-      <c r="AS14" s="176"/>
+      <c r="K14" s="158"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="123"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="114"/>
+      <c r="Q14" s="115"/>
+      <c r="R14" s="111"/>
+      <c r="S14" s="116"/>
+      <c r="T14" s="116"/>
+      <c r="U14" s="114"/>
+      <c r="V14" s="115"/>
+      <c r="W14" s="111"/>
+      <c r="X14" s="116"/>
+      <c r="Y14" s="116"/>
+      <c r="Z14" s="118"/>
+      <c r="AA14" s="119"/>
+      <c r="AB14" s="112"/>
+      <c r="AC14" s="119"/>
+      <c r="AD14" s="119"/>
+      <c r="AE14" s="118"/>
+      <c r="AF14" s="119"/>
+      <c r="AG14" s="112"/>
+      <c r="AH14" s="119"/>
+      <c r="AI14" s="119"/>
+      <c r="AJ14" s="121"/>
+      <c r="AK14" s="115"/>
+      <c r="AL14" s="116"/>
+      <c r="AM14" s="159"/>
+      <c r="AN14" s="160"/>
+      <c r="AO14" s="121"/>
+      <c r="AP14" s="115"/>
+      <c r="AQ14" s="116"/>
+      <c r="AR14" s="159"/>
+      <c r="AS14" s="160"/>
     </row>
     <row r="15" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="54">
@@ -4075,41 +4091,41 @@
       <c r="H15" s="34"/>
       <c r="I15" s="35"/>
       <c r="J15" s="67"/>
-      <c r="K15" s="174"/>
-      <c r="L15" s="126"/>
-      <c r="M15" s="139"/>
-      <c r="N15" s="128"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="130"/>
-      <c r="Q15" s="131"/>
-      <c r="R15" s="127"/>
-      <c r="S15" s="132"/>
-      <c r="T15" s="132"/>
-      <c r="U15" s="130"/>
-      <c r="V15" s="131"/>
-      <c r="W15" s="127"/>
-      <c r="X15" s="132"/>
-      <c r="Y15" s="132"/>
-      <c r="Z15" s="134"/>
-      <c r="AA15" s="135"/>
-      <c r="AB15" s="128"/>
-      <c r="AC15" s="135"/>
-      <c r="AD15" s="135"/>
-      <c r="AE15" s="134"/>
-      <c r="AF15" s="135"/>
-      <c r="AG15" s="128"/>
-      <c r="AH15" s="135"/>
-      <c r="AI15" s="135"/>
-      <c r="AJ15" s="137"/>
-      <c r="AK15" s="131"/>
-      <c r="AL15" s="132"/>
-      <c r="AM15" s="175"/>
-      <c r="AN15" s="176"/>
-      <c r="AO15" s="137"/>
-      <c r="AP15" s="131"/>
-      <c r="AQ15" s="132"/>
-      <c r="AR15" s="175"/>
-      <c r="AS15" s="176"/>
+      <c r="K15" s="158"/>
+      <c r="L15" s="110"/>
+      <c r="M15" s="123"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="113"/>
+      <c r="P15" s="114"/>
+      <c r="Q15" s="115"/>
+      <c r="R15" s="111"/>
+      <c r="S15" s="116"/>
+      <c r="T15" s="116"/>
+      <c r="U15" s="114"/>
+      <c r="V15" s="115"/>
+      <c r="W15" s="111"/>
+      <c r="X15" s="116"/>
+      <c r="Y15" s="116"/>
+      <c r="Z15" s="118"/>
+      <c r="AA15" s="119"/>
+      <c r="AB15" s="112"/>
+      <c r="AC15" s="119"/>
+      <c r="AD15" s="119"/>
+      <c r="AE15" s="118"/>
+      <c r="AF15" s="119"/>
+      <c r="AG15" s="112"/>
+      <c r="AH15" s="119"/>
+      <c r="AI15" s="119"/>
+      <c r="AJ15" s="121"/>
+      <c r="AK15" s="115"/>
+      <c r="AL15" s="116"/>
+      <c r="AM15" s="159"/>
+      <c r="AN15" s="160"/>
+      <c r="AO15" s="121"/>
+      <c r="AP15" s="115"/>
+      <c r="AQ15" s="116"/>
+      <c r="AR15" s="159"/>
+      <c r="AS15" s="160"/>
     </row>
     <row r="16" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="72">
@@ -4124,7 +4140,7 @@
       </c>
       <c r="D16" s="76">
         <f>SUM(D17:D23)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="E16" s="77"/>
       <c r="F16" s="78"/>
@@ -4132,41 +4148,41 @@
       <c r="H16" s="79"/>
       <c r="I16" s="80"/>
       <c r="J16" s="81"/>
-      <c r="K16" s="166"/>
-      <c r="L16" s="167"/>
-      <c r="M16" s="168"/>
-      <c r="N16" s="169"/>
-      <c r="O16" s="170"/>
-      <c r="P16" s="171"/>
-      <c r="Q16" s="168"/>
-      <c r="R16" s="169"/>
-      <c r="S16" s="167"/>
-      <c r="T16" s="172"/>
-      <c r="U16" s="171"/>
-      <c r="V16" s="168"/>
-      <c r="W16" s="169"/>
-      <c r="X16" s="167"/>
-      <c r="Y16" s="172"/>
-      <c r="Z16" s="171"/>
-      <c r="AA16" s="168"/>
-      <c r="AB16" s="169"/>
-      <c r="AC16" s="167"/>
-      <c r="AD16" s="172"/>
-      <c r="AE16" s="171"/>
-      <c r="AF16" s="168"/>
-      <c r="AG16" s="169"/>
-      <c r="AH16" s="167"/>
-      <c r="AI16" s="172"/>
-      <c r="AJ16" s="171"/>
-      <c r="AK16" s="168"/>
-      <c r="AL16" s="168"/>
-      <c r="AM16" s="169"/>
-      <c r="AN16" s="173"/>
-      <c r="AO16" s="171"/>
-      <c r="AP16" s="168"/>
-      <c r="AQ16" s="168"/>
-      <c r="AR16" s="169"/>
-      <c r="AS16" s="173"/>
+      <c r="K16" s="150"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="152"/>
+      <c r="N16" s="153"/>
+      <c r="O16" s="154"/>
+      <c r="P16" s="155"/>
+      <c r="Q16" s="152"/>
+      <c r="R16" s="153"/>
+      <c r="S16" s="151"/>
+      <c r="T16" s="156"/>
+      <c r="U16" s="155"/>
+      <c r="V16" s="152"/>
+      <c r="W16" s="153"/>
+      <c r="X16" s="151"/>
+      <c r="Y16" s="156"/>
+      <c r="Z16" s="155"/>
+      <c r="AA16" s="152"/>
+      <c r="AB16" s="153"/>
+      <c r="AC16" s="151"/>
+      <c r="AD16" s="156"/>
+      <c r="AE16" s="155"/>
+      <c r="AF16" s="152"/>
+      <c r="AG16" s="153"/>
+      <c r="AH16" s="151"/>
+      <c r="AI16" s="156"/>
+      <c r="AJ16" s="155"/>
+      <c r="AK16" s="152"/>
+      <c r="AL16" s="152"/>
+      <c r="AM16" s="153"/>
+      <c r="AN16" s="157"/>
+      <c r="AO16" s="155"/>
+      <c r="AP16" s="152"/>
+      <c r="AQ16" s="152"/>
+      <c r="AR16" s="153"/>
+      <c r="AS16" s="157"/>
     </row>
     <row r="17" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="54">
@@ -4178,9 +4194,9 @@
       <c r="C17" s="32">
         <v>22</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D17" s="45" t="str">
         <f t="shared" ref="D17:D22" si="1">IF(SUM(K17:AS17)=0," ",SUM(K17:AS17))</f>
-        <v>21.5</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E17" s="31">
         <v>1</v>
@@ -4192,47 +4208,41 @@
         <v>43089</v>
       </c>
       <c r="J17" s="67"/>
-      <c r="K17" s="177"/>
-      <c r="L17" s="126"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="128"/>
-      <c r="O17" s="129"/>
-      <c r="P17" s="137"/>
-      <c r="Q17" s="131"/>
-      <c r="R17" s="127"/>
-      <c r="S17" s="197">
-        <v>7</v>
-      </c>
-      <c r="T17" s="198">
-        <v>6.5</v>
-      </c>
-      <c r="U17" s="137"/>
-      <c r="V17" s="131"/>
-      <c r="W17" s="199">
-        <v>8</v>
-      </c>
-      <c r="X17" s="132"/>
-      <c r="Y17" s="133"/>
-      <c r="Z17" s="178"/>
-      <c r="AA17" s="135"/>
-      <c r="AB17" s="128"/>
-      <c r="AC17" s="135"/>
-      <c r="AD17" s="136"/>
-      <c r="AE17" s="178"/>
-      <c r="AF17" s="135"/>
-      <c r="AG17" s="128"/>
-      <c r="AH17" s="135"/>
-      <c r="AI17" s="136"/>
-      <c r="AJ17" s="137"/>
-      <c r="AK17" s="131"/>
-      <c r="AL17" s="132"/>
-      <c r="AM17" s="175"/>
-      <c r="AN17" s="176"/>
-      <c r="AO17" s="137"/>
-      <c r="AP17" s="131"/>
-      <c r="AQ17" s="132"/>
-      <c r="AR17" s="175"/>
-      <c r="AS17" s="176"/>
+      <c r="K17" s="161"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="111"/>
+      <c r="N17" s="112"/>
+      <c r="O17" s="113"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="115"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="183"/>
+      <c r="T17" s="189"/>
+      <c r="U17" s="121"/>
+      <c r="V17" s="115"/>
+      <c r="W17" s="190"/>
+      <c r="X17" s="116"/>
+      <c r="Y17" s="117"/>
+      <c r="Z17" s="162"/>
+      <c r="AA17" s="119"/>
+      <c r="AB17" s="112"/>
+      <c r="AC17" s="119"/>
+      <c r="AD17" s="120"/>
+      <c r="AE17" s="162"/>
+      <c r="AF17" s="119"/>
+      <c r="AG17" s="112"/>
+      <c r="AH17" s="119"/>
+      <c r="AI17" s="120"/>
+      <c r="AJ17" s="121"/>
+      <c r="AK17" s="115"/>
+      <c r="AL17" s="116"/>
+      <c r="AM17" s="159"/>
+      <c r="AN17" s="160"/>
+      <c r="AO17" s="121"/>
+      <c r="AP17" s="115"/>
+      <c r="AQ17" s="116"/>
+      <c r="AR17" s="159"/>
+      <c r="AS17" s="160"/>
     </row>
     <row r="18" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="54">
@@ -4244,9 +4254,9 @@
       <c r="C18" s="32">
         <v>4.5</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E18" s="31">
         <v>1</v>
@@ -4254,47 +4264,43 @@
       <c r="F18" s="32"/>
       <c r="G18" s="46"/>
       <c r="H18" s="34"/>
-      <c r="I18" s="35">
-        <v>43090</v>
-      </c>
+      <c r="I18" s="35"/>
       <c r="J18" s="67"/>
-      <c r="K18" s="177"/>
-      <c r="L18" s="126"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="128"/>
-      <c r="O18" s="129"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="131"/>
-      <c r="R18" s="127"/>
-      <c r="S18" s="132"/>
-      <c r="T18" s="133"/>
-      <c r="U18" s="137"/>
-      <c r="V18" s="131"/>
-      <c r="W18" s="127"/>
-      <c r="X18" s="197">
-        <v>4.5</v>
-      </c>
-      <c r="Y18" s="133"/>
-      <c r="Z18" s="178"/>
-      <c r="AA18" s="135"/>
-      <c r="AB18" s="128"/>
-      <c r="AC18" s="135"/>
-      <c r="AD18" s="136"/>
-      <c r="AE18" s="178"/>
-      <c r="AF18" s="135"/>
-      <c r="AG18" s="128"/>
-      <c r="AH18" s="135"/>
-      <c r="AI18" s="136"/>
-      <c r="AJ18" s="137"/>
-      <c r="AK18" s="131"/>
-      <c r="AL18" s="132"/>
-      <c r="AM18" s="175"/>
-      <c r="AN18" s="176"/>
-      <c r="AO18" s="137"/>
-      <c r="AP18" s="131"/>
-      <c r="AQ18" s="132"/>
-      <c r="AR18" s="175"/>
-      <c r="AS18" s="176"/>
+      <c r="K18" s="161"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="111"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="113"/>
+      <c r="P18" s="121"/>
+      <c r="Q18" s="115"/>
+      <c r="R18" s="111"/>
+      <c r="S18" s="116"/>
+      <c r="T18" s="117"/>
+      <c r="U18" s="121"/>
+      <c r="V18" s="115"/>
+      <c r="W18" s="111"/>
+      <c r="X18" s="183"/>
+      <c r="Y18" s="117"/>
+      <c r="Z18" s="162"/>
+      <c r="AA18" s="119"/>
+      <c r="AB18" s="112"/>
+      <c r="AC18" s="119"/>
+      <c r="AD18" s="120"/>
+      <c r="AE18" s="162"/>
+      <c r="AF18" s="119"/>
+      <c r="AG18" s="112"/>
+      <c r="AH18" s="119"/>
+      <c r="AI18" s="120"/>
+      <c r="AJ18" s="121"/>
+      <c r="AK18" s="115"/>
+      <c r="AL18" s="116"/>
+      <c r="AM18" s="159"/>
+      <c r="AN18" s="160"/>
+      <c r="AO18" s="121"/>
+      <c r="AP18" s="115"/>
+      <c r="AQ18" s="116"/>
+      <c r="AR18" s="159"/>
+      <c r="AS18" s="160"/>
     </row>
     <row r="19" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="54">
@@ -4306,9 +4312,9 @@
       <c r="C19" s="32">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E19" s="31">
         <v>1</v>
@@ -4320,59 +4326,55 @@
         <v>43091</v>
       </c>
       <c r="J19" s="67"/>
-      <c r="K19" s="177"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="127"/>
-      <c r="N19" s="128"/>
-      <c r="O19" s="129"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="131"/>
-      <c r="R19" s="127"/>
-      <c r="S19" s="132"/>
-      <c r="T19" s="133"/>
-      <c r="U19" s="137"/>
-      <c r="V19" s="131"/>
-      <c r="W19" s="127"/>
-      <c r="X19" s="197">
-        <v>3.5</v>
-      </c>
-      <c r="Y19" s="198">
-        <v>6.5</v>
-      </c>
-      <c r="Z19" s="178"/>
-      <c r="AA19" s="135"/>
-      <c r="AB19" s="128"/>
-      <c r="AC19" s="135"/>
-      <c r="AD19" s="136"/>
-      <c r="AE19" s="178"/>
-      <c r="AF19" s="135"/>
-      <c r="AG19" s="128"/>
-      <c r="AH19" s="135"/>
-      <c r="AI19" s="136"/>
-      <c r="AJ19" s="137"/>
-      <c r="AK19" s="131"/>
-      <c r="AL19" s="132"/>
-      <c r="AM19" s="175"/>
-      <c r="AN19" s="176"/>
-      <c r="AO19" s="137"/>
-      <c r="AP19" s="131"/>
-      <c r="AQ19" s="132"/>
-      <c r="AR19" s="175"/>
-      <c r="AS19" s="176"/>
+      <c r="K19" s="161"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="112"/>
+      <c r="O19" s="113"/>
+      <c r="P19" s="121"/>
+      <c r="Q19" s="115"/>
+      <c r="R19" s="111"/>
+      <c r="S19" s="116"/>
+      <c r="T19" s="117"/>
+      <c r="U19" s="121"/>
+      <c r="V19" s="115"/>
+      <c r="W19" s="111"/>
+      <c r="X19" s="183"/>
+      <c r="Y19" s="189"/>
+      <c r="Z19" s="162"/>
+      <c r="AA19" s="119"/>
+      <c r="AB19" s="112"/>
+      <c r="AC19" s="119"/>
+      <c r="AD19" s="120"/>
+      <c r="AE19" s="162"/>
+      <c r="AF19" s="119"/>
+      <c r="AG19" s="112"/>
+      <c r="AH19" s="119"/>
+      <c r="AI19" s="120"/>
+      <c r="AJ19" s="121"/>
+      <c r="AK19" s="115"/>
+      <c r="AL19" s="116"/>
+      <c r="AM19" s="159"/>
+      <c r="AN19" s="160"/>
+      <c r="AO19" s="121"/>
+      <c r="AP19" s="115"/>
+      <c r="AQ19" s="116"/>
+      <c r="AR19" s="159"/>
+      <c r="AS19" s="160"/>
     </row>
     <row r="20" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="54">
         <v>34</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C20" s="32">
         <v>1.5</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E20" s="31">
         <v>1</v>
@@ -4380,61 +4382,57 @@
       <c r="F20" s="32"/>
       <c r="G20" s="46"/>
       <c r="H20" s="34"/>
-      <c r="I20" s="35">
-        <v>42745</v>
-      </c>
+      <c r="I20" s="35"/>
       <c r="J20" s="67"/>
-      <c r="K20" s="177"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="128"/>
-      <c r="O20" s="129"/>
-      <c r="P20" s="137"/>
-      <c r="Q20" s="131"/>
-      <c r="R20" s="127"/>
-      <c r="S20" s="132"/>
-      <c r="T20" s="133"/>
-      <c r="U20" s="137"/>
-      <c r="V20" s="131"/>
-      <c r="W20" s="127"/>
-      <c r="X20" s="132"/>
-      <c r="Y20" s="133"/>
-      <c r="Z20" s="178"/>
-      <c r="AA20" s="135"/>
-      <c r="AB20" s="128"/>
-      <c r="AC20" s="135"/>
-      <c r="AD20" s="136"/>
-      <c r="AE20" s="178"/>
-      <c r="AF20" s="135"/>
-      <c r="AG20" s="128"/>
-      <c r="AH20" s="135"/>
-      <c r="AI20" s="136"/>
-      <c r="AJ20" s="137"/>
-      <c r="AK20" s="131"/>
-      <c r="AL20" s="197">
-        <v>1.5</v>
-      </c>
-      <c r="AM20" s="175"/>
-      <c r="AN20" s="176"/>
-      <c r="AO20" s="137"/>
-      <c r="AP20" s="131"/>
-      <c r="AQ20" s="132"/>
-      <c r="AR20" s="175"/>
-      <c r="AS20" s="176"/>
+      <c r="K20" s="161"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="111"/>
+      <c r="N20" s="112"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="121"/>
+      <c r="Q20" s="115"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="116"/>
+      <c r="T20" s="117"/>
+      <c r="U20" s="121"/>
+      <c r="V20" s="115"/>
+      <c r="W20" s="111"/>
+      <c r="X20" s="116"/>
+      <c r="Y20" s="117"/>
+      <c r="Z20" s="162"/>
+      <c r="AA20" s="119"/>
+      <c r="AB20" s="112"/>
+      <c r="AC20" s="119"/>
+      <c r="AD20" s="120"/>
+      <c r="AE20" s="162"/>
+      <c r="AF20" s="119"/>
+      <c r="AG20" s="112"/>
+      <c r="AH20" s="119"/>
+      <c r="AI20" s="120"/>
+      <c r="AJ20" s="121"/>
+      <c r="AK20" s="115"/>
+      <c r="AL20" s="183"/>
+      <c r="AM20" s="159"/>
+      <c r="AN20" s="160"/>
+      <c r="AO20" s="121"/>
+      <c r="AP20" s="115"/>
+      <c r="AQ20" s="116"/>
+      <c r="AR20" s="159"/>
+      <c r="AS20" s="160"/>
     </row>
     <row r="21" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="54">
         <v>35</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C21" s="32">
         <v>6.5</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E21" s="31">
         <v>2</v>
@@ -4442,61 +4440,57 @@
       <c r="F21" s="32"/>
       <c r="G21" s="46"/>
       <c r="H21" s="34"/>
-      <c r="I21" s="35">
-        <v>42745</v>
-      </c>
+      <c r="I21" s="35"/>
       <c r="J21" s="67"/>
-      <c r="K21" s="177"/>
-      <c r="L21" s="126"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="128"/>
-      <c r="O21" s="129"/>
-      <c r="P21" s="137"/>
-      <c r="Q21" s="131"/>
-      <c r="R21" s="127"/>
-      <c r="S21" s="132"/>
-      <c r="T21" s="133"/>
-      <c r="U21" s="137"/>
-      <c r="V21" s="131"/>
-      <c r="W21" s="127"/>
-      <c r="X21" s="132"/>
-      <c r="Y21" s="133"/>
-      <c r="Z21" s="178"/>
-      <c r="AA21" s="135"/>
-      <c r="AB21" s="128"/>
-      <c r="AC21" s="135"/>
-      <c r="AD21" s="136"/>
-      <c r="AE21" s="178"/>
-      <c r="AF21" s="135"/>
-      <c r="AG21" s="128"/>
-      <c r="AH21" s="135"/>
-      <c r="AI21" s="136"/>
-      <c r="AJ21" s="137"/>
-      <c r="AK21" s="131"/>
-      <c r="AL21" s="197">
-        <v>6.5</v>
-      </c>
-      <c r="AM21" s="175"/>
-      <c r="AN21" s="176"/>
-      <c r="AO21" s="137"/>
-      <c r="AP21" s="131"/>
-      <c r="AQ21" s="132"/>
-      <c r="AR21" s="175"/>
-      <c r="AS21" s="176"/>
+      <c r="K21" s="161"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="112"/>
+      <c r="O21" s="113"/>
+      <c r="P21" s="121"/>
+      <c r="Q21" s="115"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="116"/>
+      <c r="T21" s="117"/>
+      <c r="U21" s="121"/>
+      <c r="V21" s="115"/>
+      <c r="W21" s="111"/>
+      <c r="X21" s="116"/>
+      <c r="Y21" s="117"/>
+      <c r="Z21" s="162"/>
+      <c r="AA21" s="119"/>
+      <c r="AB21" s="112"/>
+      <c r="AC21" s="119"/>
+      <c r="AD21" s="120"/>
+      <c r="AE21" s="162"/>
+      <c r="AF21" s="119"/>
+      <c r="AG21" s="112"/>
+      <c r="AH21" s="119"/>
+      <c r="AI21" s="120"/>
+      <c r="AJ21" s="121"/>
+      <c r="AK21" s="115"/>
+      <c r="AL21" s="183"/>
+      <c r="AM21" s="159"/>
+      <c r="AN21" s="160"/>
+      <c r="AO21" s="121"/>
+      <c r="AP21" s="115"/>
+      <c r="AQ21" s="116"/>
+      <c r="AR21" s="159"/>
+      <c r="AS21" s="160"/>
     </row>
     <row r="22" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="54">
         <v>36</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="32">
         <v>1</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E22" s="31">
         <v>2</v>
@@ -4504,54 +4498,50 @@
       <c r="F22" s="32"/>
       <c r="G22" s="46"/>
       <c r="H22" s="34"/>
-      <c r="I22" s="35">
-        <v>42746</v>
-      </c>
+      <c r="I22" s="35"/>
       <c r="J22" s="67"/>
-      <c r="K22" s="177"/>
-      <c r="L22" s="126"/>
-      <c r="M22" s="127"/>
-      <c r="N22" s="128"/>
-      <c r="O22" s="129"/>
-      <c r="P22" s="137"/>
-      <c r="Q22" s="131"/>
-      <c r="R22" s="127"/>
-      <c r="S22" s="132"/>
-      <c r="T22" s="133"/>
-      <c r="U22" s="137"/>
-      <c r="V22" s="131"/>
-      <c r="W22" s="127"/>
-      <c r="X22" s="132"/>
-      <c r="Y22" s="133"/>
-      <c r="Z22" s="178"/>
-      <c r="AA22" s="135"/>
-      <c r="AB22" s="128"/>
-      <c r="AC22" s="135"/>
-      <c r="AD22" s="136"/>
-      <c r="AE22" s="178"/>
-      <c r="AF22" s="135"/>
-      <c r="AG22" s="128"/>
-      <c r="AH22" s="135"/>
-      <c r="AI22" s="136"/>
-      <c r="AJ22" s="137"/>
-      <c r="AK22" s="131"/>
-      <c r="AL22" s="132"/>
-      <c r="AM22" s="200">
-        <v>1</v>
-      </c>
-      <c r="AN22" s="176"/>
-      <c r="AO22" s="137"/>
-      <c r="AP22" s="131"/>
-      <c r="AQ22" s="132"/>
-      <c r="AR22" s="175"/>
-      <c r="AS22" s="176"/>
+      <c r="K22" s="161"/>
+      <c r="L22" s="110"/>
+      <c r="M22" s="111"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="113"/>
+      <c r="P22" s="121"/>
+      <c r="Q22" s="115"/>
+      <c r="R22" s="111"/>
+      <c r="S22" s="116"/>
+      <c r="T22" s="117"/>
+      <c r="U22" s="121"/>
+      <c r="V22" s="115"/>
+      <c r="W22" s="111"/>
+      <c r="X22" s="116"/>
+      <c r="Y22" s="117"/>
+      <c r="Z22" s="162"/>
+      <c r="AA22" s="119"/>
+      <c r="AB22" s="112"/>
+      <c r="AC22" s="119"/>
+      <c r="AD22" s="120"/>
+      <c r="AE22" s="162"/>
+      <c r="AF22" s="119"/>
+      <c r="AG22" s="112"/>
+      <c r="AH22" s="119"/>
+      <c r="AI22" s="120"/>
+      <c r="AJ22" s="121"/>
+      <c r="AK22" s="115"/>
+      <c r="AL22" s="116"/>
+      <c r="AM22" s="185"/>
+      <c r="AN22" s="160"/>
+      <c r="AO22" s="121"/>
+      <c r="AP22" s="115"/>
+      <c r="AQ22" s="116"/>
+      <c r="AR22" s="159"/>
+      <c r="AS22" s="160"/>
     </row>
     <row r="23" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="54">
         <v>37</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="37">
         <v>5</v>
@@ -4566,61 +4556,57 @@
       <c r="F23" s="32"/>
       <c r="G23" s="46"/>
       <c r="H23" s="34"/>
-      <c r="I23" s="35">
-        <v>42746</v>
-      </c>
+      <c r="I23" s="35"/>
       <c r="J23" s="67"/>
-      <c r="K23" s="179"/>
-      <c r="L23" s="180"/>
-      <c r="M23" s="139"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="129"/>
-      <c r="P23" s="141"/>
-      <c r="Q23" s="142"/>
-      <c r="R23" s="127"/>
-      <c r="S23" s="143"/>
-      <c r="T23" s="144"/>
-      <c r="U23" s="141"/>
-      <c r="V23" s="142"/>
-      <c r="W23" s="127"/>
-      <c r="X23" s="143"/>
-      <c r="Y23" s="144"/>
-      <c r="Z23" s="145"/>
-      <c r="AA23" s="146"/>
-      <c r="AB23" s="128"/>
-      <c r="AC23" s="146"/>
-      <c r="AD23" s="147"/>
-      <c r="AE23" s="145"/>
-      <c r="AF23" s="146"/>
-      <c r="AG23" s="128"/>
-      <c r="AH23" s="146"/>
-      <c r="AI23" s="147"/>
-      <c r="AJ23" s="181"/>
-      <c r="AK23" s="142"/>
-      <c r="AL23" s="143"/>
-      <c r="AM23" s="201">
-        <v>5</v>
-      </c>
-      <c r="AN23" s="151"/>
-      <c r="AO23" s="181"/>
-      <c r="AP23" s="142"/>
-      <c r="AQ23" s="143"/>
-      <c r="AR23" s="150"/>
-      <c r="AS23" s="151"/>
+      <c r="K23" s="163"/>
+      <c r="L23" s="164"/>
+      <c r="M23" s="123"/>
+      <c r="N23" s="124"/>
+      <c r="O23" s="113"/>
+      <c r="P23" s="125"/>
+      <c r="Q23" s="126"/>
+      <c r="R23" s="111"/>
+      <c r="S23" s="127"/>
+      <c r="T23" s="128"/>
+      <c r="U23" s="125"/>
+      <c r="V23" s="126"/>
+      <c r="W23" s="111"/>
+      <c r="X23" s="127"/>
+      <c r="Y23" s="128"/>
+      <c r="Z23" s="129"/>
+      <c r="AA23" s="130"/>
+      <c r="AB23" s="112"/>
+      <c r="AC23" s="130"/>
+      <c r="AD23" s="131"/>
+      <c r="AE23" s="129"/>
+      <c r="AF23" s="130"/>
+      <c r="AG23" s="112"/>
+      <c r="AH23" s="130"/>
+      <c r="AI23" s="131"/>
+      <c r="AJ23" s="165"/>
+      <c r="AK23" s="126"/>
+      <c r="AL23" s="127"/>
+      <c r="AM23" s="186"/>
+      <c r="AN23" s="135"/>
+      <c r="AO23" s="165"/>
+      <c r="AP23" s="126"/>
+      <c r="AQ23" s="127"/>
+      <c r="AR23" s="134"/>
+      <c r="AS23" s="135"/>
     </row>
     <row r="24" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="54">
         <v>38</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" s="32">
         <v>6.7</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="45" t="str">
         <f>IF(SUM(K24:AS24)=0," ",SUM(K24:AS24))</f>
-        <v>7</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E24" s="31">
         <v>2</v>
@@ -4632,59 +4618,55 @@
         <v>42747</v>
       </c>
       <c r="J24" s="67"/>
-      <c r="K24" s="177"/>
-      <c r="L24" s="126"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="128"/>
-      <c r="O24" s="129"/>
-      <c r="P24" s="137"/>
-      <c r="Q24" s="131"/>
-      <c r="R24" s="127"/>
-      <c r="S24" s="132"/>
-      <c r="T24" s="133"/>
-      <c r="U24" s="137"/>
-      <c r="V24" s="131"/>
-      <c r="W24" s="127"/>
-      <c r="X24" s="132"/>
-      <c r="Y24" s="133"/>
-      <c r="Z24" s="178"/>
-      <c r="AA24" s="135"/>
-      <c r="AB24" s="128"/>
-      <c r="AC24" s="135"/>
-      <c r="AD24" s="136"/>
-      <c r="AE24" s="178"/>
-      <c r="AF24" s="135"/>
-      <c r="AG24" s="128"/>
-      <c r="AH24" s="135"/>
-      <c r="AI24" s="136"/>
-      <c r="AJ24" s="137"/>
-      <c r="AK24" s="131"/>
-      <c r="AL24" s="132"/>
-      <c r="AM24" s="200">
-        <v>2</v>
-      </c>
-      <c r="AN24" s="202">
-        <v>5</v>
-      </c>
-      <c r="AO24" s="137"/>
-      <c r="AP24" s="131"/>
-      <c r="AQ24" s="132"/>
-      <c r="AR24" s="175"/>
-      <c r="AS24" s="176"/>
+      <c r="K24" s="161"/>
+      <c r="L24" s="110"/>
+      <c r="M24" s="111"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="113"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="115"/>
+      <c r="R24" s="111"/>
+      <c r="S24" s="116"/>
+      <c r="T24" s="117"/>
+      <c r="U24" s="121"/>
+      <c r="V24" s="115"/>
+      <c r="W24" s="111"/>
+      <c r="X24" s="116"/>
+      <c r="Y24" s="117"/>
+      <c r="Z24" s="162"/>
+      <c r="AA24" s="119"/>
+      <c r="AB24" s="112"/>
+      <c r="AC24" s="119"/>
+      <c r="AD24" s="120"/>
+      <c r="AE24" s="162"/>
+      <c r="AF24" s="119"/>
+      <c r="AG24" s="112"/>
+      <c r="AH24" s="119"/>
+      <c r="AI24" s="120"/>
+      <c r="AJ24" s="121"/>
+      <c r="AK24" s="115"/>
+      <c r="AL24" s="116"/>
+      <c r="AM24" s="185"/>
+      <c r="AN24" s="184"/>
+      <c r="AO24" s="121"/>
+      <c r="AP24" s="115"/>
+      <c r="AQ24" s="116"/>
+      <c r="AR24" s="159"/>
+      <c r="AS24" s="160"/>
     </row>
     <row r="25" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="54">
         <v>39</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" s="32">
         <v>3.5</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="45" t="str">
         <f>IF(SUM(K25:AS25)=0," ",SUM(K25:AS25))</f>
-        <v>3.5</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E25" s="31">
         <v>3</v>
@@ -4692,63 +4674,57 @@
       <c r="F25" s="32"/>
       <c r="G25" s="46"/>
       <c r="H25" s="34"/>
-      <c r="I25" s="35">
-        <v>42752</v>
-      </c>
+      <c r="I25" s="35"/>
       <c r="J25" s="67"/>
-      <c r="K25" s="177"/>
-      <c r="L25" s="126"/>
-      <c r="M25" s="127"/>
-      <c r="N25" s="128"/>
-      <c r="O25" s="129"/>
-      <c r="P25" s="137"/>
-      <c r="Q25" s="131"/>
-      <c r="R25" s="127"/>
-      <c r="S25" s="132"/>
-      <c r="T25" s="133"/>
-      <c r="U25" s="137"/>
-      <c r="V25" s="131"/>
-      <c r="W25" s="127"/>
-      <c r="X25" s="132"/>
-      <c r="Y25" s="133"/>
-      <c r="Z25" s="178"/>
-      <c r="AA25" s="135"/>
-      <c r="AB25" s="128"/>
-      <c r="AC25" s="135"/>
-      <c r="AD25" s="136"/>
-      <c r="AE25" s="178"/>
-      <c r="AF25" s="135"/>
-      <c r="AG25" s="128"/>
-      <c r="AH25" s="135"/>
-      <c r="AI25" s="136"/>
-      <c r="AJ25" s="137"/>
-      <c r="AK25" s="131"/>
-      <c r="AL25" s="132"/>
-      <c r="AM25" s="175"/>
-      <c r="AN25" s="202">
-        <v>1.5</v>
-      </c>
-      <c r="AO25" s="137"/>
-      <c r="AP25" s="131"/>
-      <c r="AQ25" s="197">
-        <v>2</v>
-      </c>
-      <c r="AR25" s="175"/>
-      <c r="AS25" s="176"/>
+      <c r="K25" s="161"/>
+      <c r="L25" s="110"/>
+      <c r="M25" s="111"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="113"/>
+      <c r="P25" s="121"/>
+      <c r="Q25" s="115"/>
+      <c r="R25" s="111"/>
+      <c r="S25" s="116"/>
+      <c r="T25" s="117"/>
+      <c r="U25" s="121"/>
+      <c r="V25" s="115"/>
+      <c r="W25" s="111"/>
+      <c r="X25" s="116"/>
+      <c r="Y25" s="117"/>
+      <c r="Z25" s="162"/>
+      <c r="AA25" s="119"/>
+      <c r="AB25" s="112"/>
+      <c r="AC25" s="119"/>
+      <c r="AD25" s="120"/>
+      <c r="AE25" s="162"/>
+      <c r="AF25" s="119"/>
+      <c r="AG25" s="112"/>
+      <c r="AH25" s="119"/>
+      <c r="AI25" s="120"/>
+      <c r="AJ25" s="121"/>
+      <c r="AK25" s="115"/>
+      <c r="AL25" s="116"/>
+      <c r="AM25" s="159"/>
+      <c r="AN25" s="184"/>
+      <c r="AO25" s="121"/>
+      <c r="AP25" s="115"/>
+      <c r="AQ25" s="183"/>
+      <c r="AR25" s="159"/>
+      <c r="AS25" s="160"/>
     </row>
     <row r="26" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="54">
         <v>40</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="32">
         <v>2</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="45" t="str">
         <f>IF(SUM(K26:AS26)=0," ",SUM(K26:AS26))</f>
-        <v>2</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="31">
         <v>3</v>
@@ -4756,54 +4732,50 @@
       <c r="F26" s="32"/>
       <c r="G26" s="46"/>
       <c r="H26" s="34"/>
-      <c r="I26" s="35">
-        <v>42752</v>
-      </c>
+      <c r="I26" s="35"/>
       <c r="J26" s="67"/>
-      <c r="K26" s="177"/>
-      <c r="L26" s="126"/>
-      <c r="M26" s="127"/>
-      <c r="N26" s="128"/>
-      <c r="O26" s="129"/>
-      <c r="P26" s="137"/>
-      <c r="Q26" s="131"/>
-      <c r="R26" s="127"/>
-      <c r="S26" s="132"/>
-      <c r="T26" s="133"/>
-      <c r="U26" s="137"/>
-      <c r="V26" s="131"/>
-      <c r="W26" s="127"/>
-      <c r="X26" s="132"/>
-      <c r="Y26" s="133"/>
-      <c r="Z26" s="178"/>
-      <c r="AA26" s="135"/>
-      <c r="AB26" s="128"/>
-      <c r="AC26" s="135"/>
-      <c r="AD26" s="136"/>
-      <c r="AE26" s="178"/>
-      <c r="AF26" s="135"/>
-      <c r="AG26" s="128"/>
-      <c r="AH26" s="135"/>
-      <c r="AI26" s="136"/>
-      <c r="AJ26" s="137"/>
-      <c r="AK26" s="131"/>
-      <c r="AL26" s="132"/>
-      <c r="AM26" s="175"/>
-      <c r="AN26" s="176"/>
-      <c r="AO26" s="137"/>
-      <c r="AP26" s="131"/>
-      <c r="AQ26" s="197">
-        <v>2</v>
-      </c>
-      <c r="AR26" s="175"/>
-      <c r="AS26" s="176"/>
+      <c r="K26" s="161"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="111"/>
+      <c r="N26" s="112"/>
+      <c r="O26" s="113"/>
+      <c r="P26" s="121"/>
+      <c r="Q26" s="115"/>
+      <c r="R26" s="111"/>
+      <c r="S26" s="116"/>
+      <c r="T26" s="117"/>
+      <c r="U26" s="121"/>
+      <c r="V26" s="115"/>
+      <c r="W26" s="111"/>
+      <c r="X26" s="116"/>
+      <c r="Y26" s="117"/>
+      <c r="Z26" s="162"/>
+      <c r="AA26" s="119"/>
+      <c r="AB26" s="112"/>
+      <c r="AC26" s="119"/>
+      <c r="AD26" s="120"/>
+      <c r="AE26" s="162"/>
+      <c r="AF26" s="119"/>
+      <c r="AG26" s="112"/>
+      <c r="AH26" s="119"/>
+      <c r="AI26" s="120"/>
+      <c r="AJ26" s="121"/>
+      <c r="AK26" s="115"/>
+      <c r="AL26" s="116"/>
+      <c r="AM26" s="159"/>
+      <c r="AN26" s="160"/>
+      <c r="AO26" s="121"/>
+      <c r="AP26" s="115"/>
+      <c r="AQ26" s="183"/>
+      <c r="AR26" s="159"/>
+      <c r="AS26" s="160"/>
     </row>
     <row r="27" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="54">
         <v>41</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="37">
         <v>0.5</v>
@@ -4818,54 +4790,50 @@
       <c r="F27" s="32"/>
       <c r="G27" s="46"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="35">
-        <v>42752</v>
-      </c>
+      <c r="I27" s="35"/>
       <c r="J27" s="67"/>
-      <c r="K27" s="179"/>
-      <c r="L27" s="180"/>
-      <c r="M27" s="139"/>
-      <c r="N27" s="140"/>
-      <c r="O27" s="129"/>
-      <c r="P27" s="141"/>
-      <c r="Q27" s="142"/>
-      <c r="R27" s="127"/>
-      <c r="S27" s="143"/>
-      <c r="T27" s="144"/>
-      <c r="U27" s="141"/>
-      <c r="V27" s="142"/>
-      <c r="W27" s="127"/>
-      <c r="X27" s="143"/>
-      <c r="Y27" s="144"/>
-      <c r="Z27" s="145"/>
-      <c r="AA27" s="146"/>
-      <c r="AB27" s="128"/>
-      <c r="AC27" s="146"/>
-      <c r="AD27" s="147"/>
-      <c r="AE27" s="145"/>
-      <c r="AF27" s="146"/>
-      <c r="AG27" s="128"/>
-      <c r="AH27" s="146"/>
-      <c r="AI27" s="147"/>
-      <c r="AJ27" s="181"/>
-      <c r="AK27" s="142"/>
-      <c r="AL27" s="143"/>
-      <c r="AM27" s="150"/>
-      <c r="AN27" s="151"/>
-      <c r="AO27" s="181"/>
-      <c r="AP27" s="142"/>
-      <c r="AQ27" s="195">
-        <v>0.5</v>
-      </c>
-      <c r="AR27" s="150"/>
-      <c r="AS27" s="151"/>
+      <c r="K27" s="163"/>
+      <c r="L27" s="164"/>
+      <c r="M27" s="123"/>
+      <c r="N27" s="124"/>
+      <c r="O27" s="113"/>
+      <c r="P27" s="125"/>
+      <c r="Q27" s="126"/>
+      <c r="R27" s="111"/>
+      <c r="S27" s="127"/>
+      <c r="T27" s="128"/>
+      <c r="U27" s="125"/>
+      <c r="V27" s="126"/>
+      <c r="W27" s="111"/>
+      <c r="X27" s="127"/>
+      <c r="Y27" s="128"/>
+      <c r="Z27" s="129"/>
+      <c r="AA27" s="130"/>
+      <c r="AB27" s="112"/>
+      <c r="AC27" s="130"/>
+      <c r="AD27" s="131"/>
+      <c r="AE27" s="129"/>
+      <c r="AF27" s="130"/>
+      <c r="AG27" s="112"/>
+      <c r="AH27" s="130"/>
+      <c r="AI27" s="131"/>
+      <c r="AJ27" s="165"/>
+      <c r="AK27" s="126"/>
+      <c r="AL27" s="127"/>
+      <c r="AM27" s="134"/>
+      <c r="AN27" s="135"/>
+      <c r="AO27" s="165"/>
+      <c r="AP27" s="126"/>
+      <c r="AQ27" s="181"/>
+      <c r="AR27" s="134"/>
+      <c r="AS27" s="135"/>
     </row>
     <row r="28" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="54">
         <v>42</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C28" s="37">
         <v>0.5</v>
@@ -4884,43 +4852,41 @@
         <v>42752</v>
       </c>
       <c r="J28" s="67"/>
-      <c r="K28" s="179"/>
-      <c r="L28" s="180"/>
-      <c r="M28" s="139"/>
-      <c r="N28" s="140"/>
-      <c r="O28" s="129"/>
-      <c r="P28" s="141"/>
-      <c r="Q28" s="142"/>
-      <c r="R28" s="127"/>
-      <c r="S28" s="143"/>
-      <c r="T28" s="144"/>
-      <c r="U28" s="141"/>
-      <c r="V28" s="142"/>
-      <c r="W28" s="127"/>
-      <c r="X28" s="143"/>
-      <c r="Y28" s="144"/>
-      <c r="Z28" s="145"/>
-      <c r="AA28" s="146"/>
-      <c r="AB28" s="128"/>
-      <c r="AC28" s="146"/>
-      <c r="AD28" s="147"/>
-      <c r="AE28" s="145"/>
-      <c r="AF28" s="146"/>
-      <c r="AG28" s="128"/>
-      <c r="AH28" s="146"/>
-      <c r="AI28" s="147"/>
-      <c r="AJ28" s="181"/>
-      <c r="AK28" s="142"/>
-      <c r="AL28" s="143"/>
-      <c r="AM28" s="150"/>
-      <c r="AN28" s="151"/>
-      <c r="AO28" s="181"/>
-      <c r="AP28" s="142"/>
-      <c r="AQ28" s="195">
-        <v>0.5</v>
-      </c>
-      <c r="AR28" s="150"/>
-      <c r="AS28" s="151"/>
+      <c r="K28" s="163"/>
+      <c r="L28" s="164"/>
+      <c r="M28" s="123"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="113"/>
+      <c r="P28" s="125"/>
+      <c r="Q28" s="126"/>
+      <c r="R28" s="111"/>
+      <c r="S28" s="127"/>
+      <c r="T28" s="128"/>
+      <c r="U28" s="125"/>
+      <c r="V28" s="126"/>
+      <c r="W28" s="111"/>
+      <c r="X28" s="127"/>
+      <c r="Y28" s="128"/>
+      <c r="Z28" s="129"/>
+      <c r="AA28" s="130"/>
+      <c r="AB28" s="112"/>
+      <c r="AC28" s="130"/>
+      <c r="AD28" s="131"/>
+      <c r="AE28" s="129"/>
+      <c r="AF28" s="130"/>
+      <c r="AG28" s="112"/>
+      <c r="AH28" s="130"/>
+      <c r="AI28" s="131"/>
+      <c r="AJ28" s="165"/>
+      <c r="AK28" s="126"/>
+      <c r="AL28" s="127"/>
+      <c r="AM28" s="134"/>
+      <c r="AN28" s="135"/>
+      <c r="AO28" s="165"/>
+      <c r="AP28" s="126"/>
+      <c r="AQ28" s="181"/>
+      <c r="AR28" s="134"/>
+      <c r="AS28" s="135"/>
     </row>
     <row r="29" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="72">
@@ -4943,41 +4909,41 @@
       <c r="H29" s="79"/>
       <c r="I29" s="80"/>
       <c r="J29" s="81"/>
-      <c r="K29" s="166"/>
-      <c r="L29" s="167"/>
-      <c r="M29" s="168"/>
-      <c r="N29" s="169"/>
-      <c r="O29" s="170"/>
-      <c r="P29" s="171"/>
-      <c r="Q29" s="168"/>
-      <c r="R29" s="169"/>
-      <c r="S29" s="167"/>
-      <c r="T29" s="172"/>
-      <c r="U29" s="171"/>
-      <c r="V29" s="168"/>
-      <c r="W29" s="169"/>
-      <c r="X29" s="167"/>
-      <c r="Y29" s="172"/>
-      <c r="Z29" s="171"/>
-      <c r="AA29" s="168"/>
-      <c r="AB29" s="169"/>
-      <c r="AC29" s="167"/>
-      <c r="AD29" s="172"/>
-      <c r="AE29" s="171"/>
-      <c r="AF29" s="168"/>
-      <c r="AG29" s="169"/>
-      <c r="AH29" s="167"/>
-      <c r="AI29" s="172"/>
-      <c r="AJ29" s="171"/>
-      <c r="AK29" s="168"/>
-      <c r="AL29" s="168"/>
-      <c r="AM29" s="169"/>
-      <c r="AN29" s="173"/>
-      <c r="AO29" s="171"/>
-      <c r="AP29" s="168"/>
-      <c r="AQ29" s="168"/>
-      <c r="AR29" s="169"/>
-      <c r="AS29" s="173"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="151"/>
+      <c r="M29" s="152"/>
+      <c r="N29" s="153"/>
+      <c r="O29" s="154"/>
+      <c r="P29" s="155"/>
+      <c r="Q29" s="152"/>
+      <c r="R29" s="153"/>
+      <c r="S29" s="151"/>
+      <c r="T29" s="156"/>
+      <c r="U29" s="155"/>
+      <c r="V29" s="152"/>
+      <c r="W29" s="153"/>
+      <c r="X29" s="151"/>
+      <c r="Y29" s="156"/>
+      <c r="Z29" s="155"/>
+      <c r="AA29" s="152"/>
+      <c r="AB29" s="153"/>
+      <c r="AC29" s="151"/>
+      <c r="AD29" s="156"/>
+      <c r="AE29" s="155"/>
+      <c r="AF29" s="152"/>
+      <c r="AG29" s="153"/>
+      <c r="AH29" s="151"/>
+      <c r="AI29" s="156"/>
+      <c r="AJ29" s="155"/>
+      <c r="AK29" s="152"/>
+      <c r="AL29" s="152"/>
+      <c r="AM29" s="153"/>
+      <c r="AN29" s="157"/>
+      <c r="AO29" s="155"/>
+      <c r="AP29" s="152"/>
+      <c r="AQ29" s="152"/>
+      <c r="AR29" s="153"/>
+      <c r="AS29" s="157"/>
     </row>
     <row r="30" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="54">
@@ -5001,41 +4967,41 @@
       <c r="H30" s="34"/>
       <c r="I30" s="35"/>
       <c r="J30" s="68"/>
-      <c r="K30" s="177"/>
-      <c r="L30" s="126"/>
-      <c r="M30" s="127"/>
-      <c r="N30" s="128"/>
-      <c r="O30" s="129"/>
-      <c r="P30" s="137"/>
-      <c r="Q30" s="131"/>
-      <c r="R30" s="127"/>
-      <c r="S30" s="132"/>
-      <c r="T30" s="133"/>
-      <c r="U30" s="137"/>
-      <c r="V30" s="131"/>
-      <c r="W30" s="127"/>
-      <c r="X30" s="132"/>
-      <c r="Y30" s="133"/>
-      <c r="Z30" s="178"/>
-      <c r="AA30" s="135"/>
-      <c r="AB30" s="128"/>
-      <c r="AC30" s="135"/>
-      <c r="AD30" s="136"/>
-      <c r="AE30" s="178"/>
-      <c r="AF30" s="135"/>
-      <c r="AG30" s="128"/>
-      <c r="AH30" s="135"/>
-      <c r="AI30" s="136"/>
-      <c r="AJ30" s="137"/>
-      <c r="AK30" s="131"/>
-      <c r="AL30" s="132"/>
-      <c r="AM30" s="132"/>
-      <c r="AN30" s="182"/>
-      <c r="AO30" s="137"/>
-      <c r="AP30" s="131"/>
-      <c r="AQ30" s="132"/>
-      <c r="AR30" s="132"/>
-      <c r="AS30" s="182"/>
+      <c r="K30" s="161"/>
+      <c r="L30" s="110"/>
+      <c r="M30" s="111"/>
+      <c r="N30" s="112"/>
+      <c r="O30" s="113"/>
+      <c r="P30" s="121"/>
+      <c r="Q30" s="115"/>
+      <c r="R30" s="111"/>
+      <c r="S30" s="116"/>
+      <c r="T30" s="117"/>
+      <c r="U30" s="121"/>
+      <c r="V30" s="115"/>
+      <c r="W30" s="111"/>
+      <c r="X30" s="116"/>
+      <c r="Y30" s="117"/>
+      <c r="Z30" s="162"/>
+      <c r="AA30" s="119"/>
+      <c r="AB30" s="112"/>
+      <c r="AC30" s="119"/>
+      <c r="AD30" s="120"/>
+      <c r="AE30" s="162"/>
+      <c r="AF30" s="119"/>
+      <c r="AG30" s="112"/>
+      <c r="AH30" s="119"/>
+      <c r="AI30" s="120"/>
+      <c r="AJ30" s="121"/>
+      <c r="AK30" s="115"/>
+      <c r="AL30" s="116"/>
+      <c r="AM30" s="116"/>
+      <c r="AN30" s="166"/>
+      <c r="AO30" s="121"/>
+      <c r="AP30" s="115"/>
+      <c r="AQ30" s="116"/>
+      <c r="AR30" s="116"/>
+      <c r="AS30" s="166"/>
     </row>
     <row r="31" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="54">
@@ -5059,41 +5025,41 @@
       <c r="H31" s="34"/>
       <c r="I31" s="35"/>
       <c r="J31" s="68"/>
-      <c r="K31" s="177"/>
-      <c r="L31" s="126"/>
-      <c r="M31" s="127"/>
-      <c r="N31" s="128"/>
-      <c r="O31" s="129"/>
-      <c r="P31" s="137"/>
-      <c r="Q31" s="131"/>
-      <c r="R31" s="127"/>
-      <c r="S31" s="132"/>
-      <c r="T31" s="133"/>
-      <c r="U31" s="137"/>
-      <c r="V31" s="131"/>
-      <c r="W31" s="127"/>
-      <c r="X31" s="132"/>
-      <c r="Y31" s="133"/>
-      <c r="Z31" s="178"/>
-      <c r="AA31" s="135"/>
-      <c r="AB31" s="128"/>
-      <c r="AC31" s="135"/>
-      <c r="AD31" s="136"/>
-      <c r="AE31" s="178"/>
-      <c r="AF31" s="135"/>
-      <c r="AG31" s="128"/>
-      <c r="AH31" s="135"/>
-      <c r="AI31" s="136"/>
-      <c r="AJ31" s="137"/>
-      <c r="AK31" s="142"/>
-      <c r="AL31" s="143"/>
-      <c r="AM31" s="143"/>
-      <c r="AN31" s="183"/>
-      <c r="AO31" s="137"/>
-      <c r="AP31" s="142"/>
-      <c r="AQ31" s="143"/>
-      <c r="AR31" s="143"/>
-      <c r="AS31" s="183"/>
+      <c r="K31" s="161"/>
+      <c r="L31" s="110"/>
+      <c r="M31" s="111"/>
+      <c r="N31" s="112"/>
+      <c r="O31" s="113"/>
+      <c r="P31" s="121"/>
+      <c r="Q31" s="115"/>
+      <c r="R31" s="111"/>
+      <c r="S31" s="116"/>
+      <c r="T31" s="117"/>
+      <c r="U31" s="121"/>
+      <c r="V31" s="115"/>
+      <c r="W31" s="111"/>
+      <c r="X31" s="116"/>
+      <c r="Y31" s="117"/>
+      <c r="Z31" s="162"/>
+      <c r="AA31" s="119"/>
+      <c r="AB31" s="112"/>
+      <c r="AC31" s="119"/>
+      <c r="AD31" s="120"/>
+      <c r="AE31" s="162"/>
+      <c r="AF31" s="119"/>
+      <c r="AG31" s="112"/>
+      <c r="AH31" s="119"/>
+      <c r="AI31" s="120"/>
+      <c r="AJ31" s="121"/>
+      <c r="AK31" s="126"/>
+      <c r="AL31" s="127"/>
+      <c r="AM31" s="127"/>
+      <c r="AN31" s="167"/>
+      <c r="AO31" s="121"/>
+      <c r="AP31" s="126"/>
+      <c r="AQ31" s="127"/>
+      <c r="AR31" s="127"/>
+      <c r="AS31" s="167"/>
     </row>
     <row r="32" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="54">
@@ -5117,41 +5083,41 @@
       <c r="H32" s="39"/>
       <c r="I32" s="35"/>
       <c r="J32" s="68"/>
-      <c r="K32" s="179"/>
-      <c r="L32" s="180"/>
-      <c r="M32" s="139"/>
-      <c r="N32" s="140"/>
-      <c r="O32" s="154"/>
-      <c r="P32" s="184"/>
-      <c r="Q32" s="185"/>
-      <c r="R32" s="139"/>
-      <c r="S32" s="186"/>
-      <c r="T32" s="187"/>
-      <c r="U32" s="184"/>
-      <c r="V32" s="185"/>
-      <c r="W32" s="139"/>
-      <c r="X32" s="186"/>
-      <c r="Y32" s="187"/>
-      <c r="Z32" s="188"/>
-      <c r="AA32" s="189"/>
-      <c r="AB32" s="140"/>
-      <c r="AC32" s="189"/>
-      <c r="AD32" s="190"/>
-      <c r="AE32" s="188"/>
-      <c r="AF32" s="189"/>
-      <c r="AG32" s="140"/>
-      <c r="AH32" s="189"/>
-      <c r="AI32" s="190"/>
-      <c r="AJ32" s="184"/>
-      <c r="AK32" s="131"/>
-      <c r="AL32" s="132"/>
-      <c r="AM32" s="132"/>
-      <c r="AN32" s="149"/>
-      <c r="AO32" s="184"/>
-      <c r="AP32" s="131"/>
-      <c r="AQ32" s="132"/>
-      <c r="AR32" s="132"/>
-      <c r="AS32" s="149"/>
+      <c r="K32" s="163"/>
+      <c r="L32" s="164"/>
+      <c r="M32" s="123"/>
+      <c r="N32" s="124"/>
+      <c r="O32" s="138"/>
+      <c r="P32" s="168"/>
+      <c r="Q32" s="169"/>
+      <c r="R32" s="123"/>
+      <c r="S32" s="170"/>
+      <c r="T32" s="171"/>
+      <c r="U32" s="168"/>
+      <c r="V32" s="169"/>
+      <c r="W32" s="123"/>
+      <c r="X32" s="170"/>
+      <c r="Y32" s="171"/>
+      <c r="Z32" s="172"/>
+      <c r="AA32" s="173"/>
+      <c r="AB32" s="124"/>
+      <c r="AC32" s="173"/>
+      <c r="AD32" s="174"/>
+      <c r="AE32" s="172"/>
+      <c r="AF32" s="173"/>
+      <c r="AG32" s="124"/>
+      <c r="AH32" s="173"/>
+      <c r="AI32" s="174"/>
+      <c r="AJ32" s="168"/>
+      <c r="AK32" s="115"/>
+      <c r="AL32" s="116"/>
+      <c r="AM32" s="116"/>
+      <c r="AN32" s="133"/>
+      <c r="AO32" s="168"/>
+      <c r="AP32" s="115"/>
+      <c r="AQ32" s="116"/>
+      <c r="AR32" s="116"/>
+      <c r="AS32" s="133"/>
     </row>
     <row r="33" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="72">
@@ -5174,41 +5140,41 @@
       <c r="H33" s="79"/>
       <c r="I33" s="80"/>
       <c r="J33" s="81"/>
-      <c r="K33" s="166"/>
-      <c r="L33" s="167"/>
-      <c r="M33" s="168"/>
-      <c r="N33" s="169"/>
-      <c r="O33" s="170"/>
-      <c r="P33" s="171"/>
-      <c r="Q33" s="168"/>
-      <c r="R33" s="169"/>
-      <c r="S33" s="167"/>
-      <c r="T33" s="172"/>
-      <c r="U33" s="171"/>
-      <c r="V33" s="168"/>
-      <c r="W33" s="169"/>
-      <c r="X33" s="167"/>
-      <c r="Y33" s="172"/>
-      <c r="Z33" s="171"/>
-      <c r="AA33" s="168"/>
-      <c r="AB33" s="169"/>
-      <c r="AC33" s="167"/>
-      <c r="AD33" s="172"/>
-      <c r="AE33" s="171"/>
-      <c r="AF33" s="168"/>
-      <c r="AG33" s="169"/>
-      <c r="AH33" s="167"/>
-      <c r="AI33" s="172"/>
-      <c r="AJ33" s="171"/>
-      <c r="AK33" s="168"/>
-      <c r="AL33" s="168"/>
-      <c r="AM33" s="169"/>
-      <c r="AN33" s="173"/>
-      <c r="AO33" s="171"/>
-      <c r="AP33" s="168"/>
-      <c r="AQ33" s="168"/>
-      <c r="AR33" s="169"/>
-      <c r="AS33" s="173"/>
+      <c r="K33" s="150"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="152"/>
+      <c r="N33" s="153"/>
+      <c r="O33" s="154"/>
+      <c r="P33" s="155"/>
+      <c r="Q33" s="152"/>
+      <c r="R33" s="153"/>
+      <c r="S33" s="151"/>
+      <c r="T33" s="156"/>
+      <c r="U33" s="155"/>
+      <c r="V33" s="152"/>
+      <c r="W33" s="153"/>
+      <c r="X33" s="151"/>
+      <c r="Y33" s="156"/>
+      <c r="Z33" s="155"/>
+      <c r="AA33" s="152"/>
+      <c r="AB33" s="153"/>
+      <c r="AC33" s="151"/>
+      <c r="AD33" s="156"/>
+      <c r="AE33" s="155"/>
+      <c r="AF33" s="152"/>
+      <c r="AG33" s="153"/>
+      <c r="AH33" s="151"/>
+      <c r="AI33" s="156"/>
+      <c r="AJ33" s="155"/>
+      <c r="AK33" s="152"/>
+      <c r="AL33" s="152"/>
+      <c r="AM33" s="153"/>
+      <c r="AN33" s="157"/>
+      <c r="AO33" s="155"/>
+      <c r="AP33" s="152"/>
+      <c r="AQ33" s="152"/>
+      <c r="AR33" s="153"/>
+      <c r="AS33" s="157"/>
     </row>
     <row r="34" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="55">
@@ -5229,47 +5195,41 @@
       <c r="H34" s="34"/>
       <c r="I34" s="35"/>
       <c r="J34" s="68"/>
-      <c r="K34" s="177"/>
-      <c r="L34" s="126"/>
-      <c r="M34" s="127"/>
-      <c r="N34" s="128"/>
-      <c r="O34" s="129"/>
-      <c r="P34" s="137"/>
-      <c r="Q34" s="131"/>
-      <c r="R34" s="199">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="S34" s="197">
-        <v>0.7</v>
-      </c>
-      <c r="T34" s="133"/>
-      <c r="U34" s="137"/>
-      <c r="V34" s="131"/>
-      <c r="W34" s="127"/>
-      <c r="X34" s="132"/>
-      <c r="Y34" s="133"/>
-      <c r="Z34" s="178"/>
-      <c r="AA34" s="135"/>
-      <c r="AB34" s="128"/>
-      <c r="AC34" s="135"/>
-      <c r="AD34" s="136"/>
-      <c r="AE34" s="178"/>
-      <c r="AF34" s="135"/>
-      <c r="AG34" s="128"/>
-      <c r="AH34" s="135"/>
-      <c r="AI34" s="136"/>
-      <c r="AJ34" s="137"/>
-      <c r="AK34" s="131"/>
-      <c r="AL34" s="132"/>
-      <c r="AM34" s="132"/>
-      <c r="AN34" s="182"/>
-      <c r="AO34" s="137"/>
-      <c r="AP34" s="131"/>
-      <c r="AQ34" s="197">
-        <v>3</v>
-      </c>
-      <c r="AR34" s="132"/>
-      <c r="AS34" s="182"/>
+      <c r="K34" s="161"/>
+      <c r="L34" s="110"/>
+      <c r="M34" s="111"/>
+      <c r="N34" s="112"/>
+      <c r="O34" s="113"/>
+      <c r="P34" s="121"/>
+      <c r="Q34" s="115"/>
+      <c r="R34" s="190"/>
+      <c r="S34" s="183"/>
+      <c r="T34" s="117"/>
+      <c r="U34" s="121"/>
+      <c r="V34" s="115"/>
+      <c r="W34" s="111"/>
+      <c r="X34" s="116"/>
+      <c r="Y34" s="117"/>
+      <c r="Z34" s="162"/>
+      <c r="AA34" s="119"/>
+      <c r="AB34" s="112"/>
+      <c r="AC34" s="119"/>
+      <c r="AD34" s="120"/>
+      <c r="AE34" s="162"/>
+      <c r="AF34" s="119"/>
+      <c r="AG34" s="112"/>
+      <c r="AH34" s="119"/>
+      <c r="AI34" s="120"/>
+      <c r="AJ34" s="121"/>
+      <c r="AK34" s="115"/>
+      <c r="AL34" s="116"/>
+      <c r="AM34" s="116"/>
+      <c r="AN34" s="166"/>
+      <c r="AO34" s="121"/>
+      <c r="AP34" s="115"/>
+      <c r="AQ34" s="183"/>
+      <c r="AR34" s="116"/>
+      <c r="AS34" s="166"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="55">
@@ -5287,41 +5247,41 @@
       <c r="H35" s="44"/>
       <c r="I35" s="35"/>
       <c r="J35" s="67"/>
-      <c r="K35" s="191"/>
-      <c r="L35" s="192"/>
-      <c r="M35" s="157"/>
-      <c r="N35" s="162"/>
-      <c r="O35" s="154"/>
-      <c r="P35" s="184"/>
-      <c r="Q35" s="185"/>
-      <c r="R35" s="157"/>
-      <c r="S35" s="186"/>
-      <c r="T35" s="187"/>
-      <c r="U35" s="184"/>
-      <c r="V35" s="185"/>
-      <c r="W35" s="157"/>
-      <c r="X35" s="186"/>
-      <c r="Y35" s="187"/>
-      <c r="Z35" s="188"/>
-      <c r="AA35" s="189"/>
-      <c r="AB35" s="162"/>
-      <c r="AC35" s="189"/>
-      <c r="AD35" s="190"/>
-      <c r="AE35" s="188"/>
-      <c r="AF35" s="189"/>
-      <c r="AG35" s="162"/>
-      <c r="AH35" s="189"/>
-      <c r="AI35" s="190"/>
-      <c r="AJ35" s="193"/>
-      <c r="AK35" s="185"/>
-      <c r="AL35" s="186"/>
-      <c r="AM35" s="186"/>
-      <c r="AN35" s="149"/>
-      <c r="AO35" s="193"/>
-      <c r="AP35" s="185"/>
-      <c r="AQ35" s="186"/>
-      <c r="AR35" s="186"/>
-      <c r="AS35" s="149"/>
+      <c r="K35" s="175"/>
+      <c r="L35" s="176"/>
+      <c r="M35" s="141"/>
+      <c r="N35" s="146"/>
+      <c r="O35" s="138"/>
+      <c r="P35" s="168"/>
+      <c r="Q35" s="169"/>
+      <c r="R35" s="141"/>
+      <c r="S35" s="170"/>
+      <c r="T35" s="171"/>
+      <c r="U35" s="168"/>
+      <c r="V35" s="169"/>
+      <c r="W35" s="141"/>
+      <c r="X35" s="170"/>
+      <c r="Y35" s="171"/>
+      <c r="Z35" s="172"/>
+      <c r="AA35" s="173"/>
+      <c r="AB35" s="146"/>
+      <c r="AC35" s="173"/>
+      <c r="AD35" s="174"/>
+      <c r="AE35" s="172"/>
+      <c r="AF35" s="173"/>
+      <c r="AG35" s="146"/>
+      <c r="AH35" s="173"/>
+      <c r="AI35" s="174"/>
+      <c r="AJ35" s="177"/>
+      <c r="AK35" s="169"/>
+      <c r="AL35" s="170"/>
+      <c r="AM35" s="170"/>
+      <c r="AN35" s="133"/>
+      <c r="AO35" s="177"/>
+      <c r="AP35" s="169"/>
+      <c r="AQ35" s="170"/>
+      <c r="AR35" s="170"/>
+      <c r="AS35" s="133"/>
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="72">
@@ -5344,41 +5304,41 @@
       <c r="H36" s="79"/>
       <c r="I36" s="80"/>
       <c r="J36" s="81"/>
-      <c r="K36" s="166"/>
-      <c r="L36" s="167"/>
-      <c r="M36" s="168"/>
-      <c r="N36" s="169"/>
-      <c r="O36" s="170"/>
-      <c r="P36" s="171"/>
-      <c r="Q36" s="168"/>
-      <c r="R36" s="169"/>
-      <c r="S36" s="167"/>
-      <c r="T36" s="172"/>
-      <c r="U36" s="171"/>
-      <c r="V36" s="168"/>
-      <c r="W36" s="169"/>
-      <c r="X36" s="167"/>
-      <c r="Y36" s="172"/>
-      <c r="Z36" s="171"/>
-      <c r="AA36" s="168"/>
-      <c r="AB36" s="169"/>
-      <c r="AC36" s="167"/>
-      <c r="AD36" s="172"/>
-      <c r="AE36" s="171"/>
-      <c r="AF36" s="168"/>
-      <c r="AG36" s="169"/>
-      <c r="AH36" s="167"/>
-      <c r="AI36" s="172"/>
-      <c r="AJ36" s="171"/>
-      <c r="AK36" s="168"/>
-      <c r="AL36" s="168"/>
-      <c r="AM36" s="169"/>
-      <c r="AN36" s="173"/>
-      <c r="AO36" s="171"/>
-      <c r="AP36" s="168"/>
-      <c r="AQ36" s="168"/>
-      <c r="AR36" s="169"/>
-      <c r="AS36" s="173"/>
+      <c r="K36" s="150"/>
+      <c r="L36" s="151"/>
+      <c r="M36" s="152"/>
+      <c r="N36" s="153"/>
+      <c r="O36" s="154"/>
+      <c r="P36" s="155"/>
+      <c r="Q36" s="152"/>
+      <c r="R36" s="153"/>
+      <c r="S36" s="151"/>
+      <c r="T36" s="156"/>
+      <c r="U36" s="155"/>
+      <c r="V36" s="152"/>
+      <c r="W36" s="153"/>
+      <c r="X36" s="151"/>
+      <c r="Y36" s="156"/>
+      <c r="Z36" s="155"/>
+      <c r="AA36" s="152"/>
+      <c r="AB36" s="153"/>
+      <c r="AC36" s="151"/>
+      <c r="AD36" s="156"/>
+      <c r="AE36" s="155"/>
+      <c r="AF36" s="152"/>
+      <c r="AG36" s="153"/>
+      <c r="AH36" s="151"/>
+      <c r="AI36" s="156"/>
+      <c r="AJ36" s="155"/>
+      <c r="AK36" s="152"/>
+      <c r="AL36" s="152"/>
+      <c r="AM36" s="153"/>
+      <c r="AN36" s="157"/>
+      <c r="AO36" s="155"/>
+      <c r="AP36" s="152"/>
+      <c r="AQ36" s="152"/>
+      <c r="AR36" s="153"/>
+      <c r="AS36" s="157"/>
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="54">
@@ -5400,48 +5360,48 @@
       <c r="H37" s="34"/>
       <c r="I37" s="35"/>
       <c r="J37" s="70"/>
-      <c r="K37" s="177"/>
-      <c r="L37" s="126"/>
-      <c r="M37" s="127"/>
-      <c r="N37" s="128"/>
-      <c r="O37" s="129"/>
-      <c r="P37" s="137"/>
-      <c r="Q37" s="131"/>
-      <c r="R37" s="127"/>
-      <c r="S37" s="132"/>
-      <c r="T37" s="133"/>
-      <c r="U37" s="137"/>
-      <c r="V37" s="131"/>
-      <c r="W37" s="127"/>
-      <c r="X37" s="132"/>
-      <c r="Y37" s="133"/>
-      <c r="Z37" s="178"/>
-      <c r="AA37" s="135"/>
-      <c r="AB37" s="128"/>
-      <c r="AC37" s="135"/>
-      <c r="AD37" s="136"/>
-      <c r="AE37" s="178"/>
-      <c r="AF37" s="135"/>
-      <c r="AG37" s="128"/>
-      <c r="AH37" s="135"/>
-      <c r="AI37" s="136"/>
-      <c r="AJ37" s="130"/>
-      <c r="AK37" s="131"/>
-      <c r="AL37" s="132"/>
-      <c r="AM37" s="132"/>
-      <c r="AN37" s="183"/>
-      <c r="AO37" s="130"/>
-      <c r="AP37" s="131"/>
-      <c r="AQ37" s="132"/>
-      <c r="AR37" s="132"/>
-      <c r="AS37" s="183"/>
+      <c r="K37" s="161"/>
+      <c r="L37" s="110"/>
+      <c r="M37" s="111"/>
+      <c r="N37" s="112"/>
+      <c r="O37" s="113"/>
+      <c r="P37" s="121"/>
+      <c r="Q37" s="115"/>
+      <c r="R37" s="111"/>
+      <c r="S37" s="116"/>
+      <c r="T37" s="117"/>
+      <c r="U37" s="121"/>
+      <c r="V37" s="115"/>
+      <c r="W37" s="111"/>
+      <c r="X37" s="116"/>
+      <c r="Y37" s="117"/>
+      <c r="Z37" s="162"/>
+      <c r="AA37" s="119"/>
+      <c r="AB37" s="112"/>
+      <c r="AC37" s="119"/>
+      <c r="AD37" s="120"/>
+      <c r="AE37" s="162"/>
+      <c r="AF37" s="119"/>
+      <c r="AG37" s="112"/>
+      <c r="AH37" s="119"/>
+      <c r="AI37" s="120"/>
+      <c r="AJ37" s="114"/>
+      <c r="AK37" s="115"/>
+      <c r="AL37" s="116"/>
+      <c r="AM37" s="116"/>
+      <c r="AN37" s="167"/>
+      <c r="AO37" s="114"/>
+      <c r="AP37" s="115"/>
+      <c r="AQ37" s="116"/>
+      <c r="AR37" s="116"/>
+      <c r="AS37" s="167"/>
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="53">
         <v>72</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="33" t="str">
@@ -5458,41 +5418,41 @@
         <v>43118</v>
       </c>
       <c r="J38" s="69"/>
-      <c r="K38" s="179"/>
-      <c r="L38" s="180"/>
-      <c r="M38" s="139"/>
-      <c r="N38" s="140"/>
-      <c r="O38" s="129"/>
-      <c r="P38" s="181"/>
-      <c r="Q38" s="142"/>
-      <c r="R38" s="127"/>
-      <c r="S38" s="143"/>
-      <c r="T38" s="144"/>
-      <c r="U38" s="181"/>
-      <c r="V38" s="142"/>
-      <c r="W38" s="127"/>
-      <c r="X38" s="143"/>
-      <c r="Y38" s="144"/>
-      <c r="Z38" s="194"/>
-      <c r="AA38" s="146"/>
-      <c r="AB38" s="128"/>
-      <c r="AC38" s="146"/>
-      <c r="AD38" s="147"/>
-      <c r="AE38" s="194"/>
-      <c r="AF38" s="146"/>
-      <c r="AG38" s="128"/>
-      <c r="AH38" s="146"/>
-      <c r="AI38" s="147"/>
-      <c r="AJ38" s="141"/>
-      <c r="AK38" s="142"/>
-      <c r="AL38" s="143"/>
-      <c r="AM38" s="143"/>
-      <c r="AN38" s="183"/>
-      <c r="AO38" s="141"/>
-      <c r="AP38" s="142"/>
-      <c r="AQ38" s="143"/>
-      <c r="AR38" s="143"/>
-      <c r="AS38" s="183"/>
+      <c r="K38" s="163"/>
+      <c r="L38" s="164"/>
+      <c r="M38" s="123"/>
+      <c r="N38" s="124"/>
+      <c r="O38" s="113"/>
+      <c r="P38" s="165"/>
+      <c r="Q38" s="126"/>
+      <c r="R38" s="111"/>
+      <c r="S38" s="127"/>
+      <c r="T38" s="128"/>
+      <c r="U38" s="165"/>
+      <c r="V38" s="126"/>
+      <c r="W38" s="111"/>
+      <c r="X38" s="127"/>
+      <c r="Y38" s="128"/>
+      <c r="Z38" s="178"/>
+      <c r="AA38" s="130"/>
+      <c r="AB38" s="112"/>
+      <c r="AC38" s="130"/>
+      <c r="AD38" s="131"/>
+      <c r="AE38" s="178"/>
+      <c r="AF38" s="130"/>
+      <c r="AG38" s="112"/>
+      <c r="AH38" s="130"/>
+      <c r="AI38" s="131"/>
+      <c r="AJ38" s="125"/>
+      <c r="AK38" s="126"/>
+      <c r="AL38" s="127"/>
+      <c r="AM38" s="127"/>
+      <c r="AN38" s="167"/>
+      <c r="AO38" s="125"/>
+      <c r="AP38" s="126"/>
+      <c r="AQ38" s="127"/>
+      <c r="AR38" s="127"/>
+      <c r="AS38" s="167"/>
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="71"/>
@@ -5501,11 +5461,11 @@
       </c>
       <c r="C39" s="90">
         <f>SUM(C5+C11+C16+C29+C33+C36)</f>
-        <v>96.4</v>
+        <v>102.4</v>
       </c>
       <c r="D39" s="90">
         <f>SUM(D36+D33+D29+D16+D11+D5)</f>
-        <v>63.7</v>
+        <v>14.4</v>
       </c>
       <c r="E39" s="90"/>
       <c r="F39" s="90"/>
@@ -5543,15 +5503,15 @@
       </c>
       <c r="R39" s="94">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>6.9</v>
       </c>
       <c r="S39" s="90">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="T39" s="94">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U39" s="94">
         <f t="shared" si="2"/>
@@ -5563,15 +5523,15 @@
       </c>
       <c r="W39" s="94">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="X39" s="90">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y39" s="94">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Z39" s="94">
         <f t="shared" si="2"/>
@@ -5623,15 +5583,15 @@
       </c>
       <c r="AL39" s="94">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM39" s="90">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AN39" s="95">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AO39" s="94">
         <f t="shared" si="2"/>
@@ -5643,7 +5603,7 @@
       </c>
       <c r="AQ39" s="94">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AR39" s="90">
         <f t="shared" si="2"/>
@@ -5656,15 +5616,15 @@
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="96"/>
-      <c r="B40" s="108"/>
-      <c r="C40" s="108"/>
-      <c r="D40" s="108"/>
-      <c r="E40" s="108"/>
-      <c r="F40" s="108"/>
-      <c r="G40" s="108"/>
-      <c r="H40" s="108"/>
-      <c r="I40" s="108"/>
-      <c r="J40" s="108"/>
+      <c r="B40" s="193"/>
+      <c r="C40" s="193"/>
+      <c r="D40" s="193"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="107"/>
@@ -5679,26 +5639,26 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
-      <c r="K41" s="115"/>
-      <c r="L41" s="116"/>
-      <c r="M41" s="116"/>
-      <c r="N41" s="116"/>
-      <c r="O41" s="116"/>
-      <c r="P41" s="116"/>
-      <c r="Q41" s="116"/>
-      <c r="R41" s="116"/>
-      <c r="S41" s="116"/>
-      <c r="T41" s="116"/>
-      <c r="U41" s="116"/>
-      <c r="V41" s="116"/>
-      <c r="W41" s="116"/>
-      <c r="X41" s="116"/>
-      <c r="Y41" s="116"/>
-      <c r="Z41" s="116"/>
-      <c r="AA41" s="116"/>
-      <c r="AB41" s="116"/>
-      <c r="AC41" s="116"/>
-      <c r="AD41" s="116"/>
+      <c r="K41" s="200"/>
+      <c r="L41" s="201"/>
+      <c r="M41" s="201"/>
+      <c r="N41" s="201"/>
+      <c r="O41" s="201"/>
+      <c r="P41" s="201"/>
+      <c r="Q41" s="201"/>
+      <c r="R41" s="201"/>
+      <c r="S41" s="201"/>
+      <c r="T41" s="201"/>
+      <c r="U41" s="201"/>
+      <c r="V41" s="201"/>
+      <c r="W41" s="201"/>
+      <c r="X41" s="201"/>
+      <c r="Y41" s="201"/>
+      <c r="Z41" s="201"/>
+      <c r="AA41" s="201"/>
+      <c r="AB41" s="201"/>
+      <c r="AC41" s="201"/>
+      <c r="AD41" s="201"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="106"/>
@@ -5713,31 +5673,31 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
-      <c r="K42" s="114"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="114"/>
-      <c r="N42" s="114"/>
-      <c r="O42" s="114"/>
-      <c r="P42" s="114"/>
-      <c r="Q42" s="114"/>
-      <c r="R42" s="114"/>
-      <c r="S42" s="114"/>
-      <c r="T42" s="114"/>
-      <c r="U42" s="114"/>
-      <c r="V42" s="114"/>
-      <c r="W42" s="114"/>
-      <c r="X42" s="114"/>
-      <c r="Y42" s="114"/>
-      <c r="Z42" s="114"/>
-      <c r="AA42" s="114"/>
-      <c r="AB42" s="114"/>
-      <c r="AC42" s="114"/>
-      <c r="AD42" s="114"/>
+      <c r="K42" s="199"/>
+      <c r="L42" s="199"/>
+      <c r="M42" s="199"/>
+      <c r="N42" s="199"/>
+      <c r="O42" s="199"/>
+      <c r="P42" s="199"/>
+      <c r="Q42" s="199"/>
+      <c r="R42" s="199"/>
+      <c r="S42" s="199"/>
+      <c r="T42" s="199"/>
+      <c r="U42" s="199"/>
+      <c r="V42" s="199"/>
+      <c r="W42" s="199"/>
+      <c r="X42" s="199"/>
+      <c r="Y42" s="199"/>
+      <c r="Z42" s="199"/>
+      <c r="AA42" s="199"/>
+      <c r="AB42" s="199"/>
+      <c r="AC42" s="199"/>
+      <c r="AD42" s="199"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="124"/>
+      <c r="A43" s="108"/>
       <c r="B43" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="13"/>
@@ -5747,28 +5707,32 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114"/>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-      <c r="O43" s="114"/>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="114"/>
-      <c r="S43" s="114"/>
-      <c r="T43" s="114"/>
-      <c r="U43" s="114"/>
-      <c r="V43" s="114"/>
-      <c r="W43" s="114"/>
-      <c r="X43" s="114"/>
-      <c r="Y43" s="114"/>
-      <c r="Z43" s="114"/>
-      <c r="AA43" s="114"/>
-      <c r="AB43" s="114"/>
-      <c r="AC43" s="114"/>
-      <c r="AD43" s="114"/>
+      <c r="K43" s="199"/>
+      <c r="L43" s="199"/>
+      <c r="M43" s="199"/>
+      <c r="N43" s="199"/>
+      <c r="O43" s="199"/>
+      <c r="P43" s="199"/>
+      <c r="Q43" s="199"/>
+      <c r="R43" s="199"/>
+      <c r="S43" s="199"/>
+      <c r="T43" s="199"/>
+      <c r="U43" s="199"/>
+      <c r="V43" s="199"/>
+      <c r="W43" s="199"/>
+      <c r="X43" s="199"/>
+      <c r="Y43" s="199"/>
+      <c r="Z43" s="199"/>
+      <c r="AA43" s="199"/>
+      <c r="AB43" s="199"/>
+      <c r="AC43" s="199"/>
+      <c r="AD43" s="199"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="182"/>
+      <c r="B44" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="J44" s="5"/>
     </row>
   </sheetData>
@@ -5804,8 +5768,8 @@
   </sheetPr>
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B38"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5817,20 +5781,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="119"/>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
+      <c r="A1" s="204"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
+      <c r="M1" s="204"/>
+      <c r="N1" s="204"/>
     </row>
     <row r="2" spans="1:14" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="100"/>
@@ -5933,7 +5897,7 @@
       </c>
       <c r="B11" s="101">
         <f>Zeitplanung!R39</f>
-        <v>8</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5943,7 +5907,7 @@
       </c>
       <c r="B12" s="101">
         <f>Zeitplanung!S39</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5953,7 +5917,7 @@
       </c>
       <c r="B13" s="101">
         <f>Zeitplanung!T39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5983,7 +5947,7 @@
       </c>
       <c r="B16" s="101">
         <f>Zeitplanung!W39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5993,7 +5957,7 @@
       </c>
       <c r="B17" s="101">
         <f>Zeitplanung!X39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -6003,7 +5967,7 @@
       </c>
       <c r="B18" s="101">
         <f>Zeitplanung!Y39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -6133,7 +6097,7 @@
       </c>
       <c r="B31" s="101">
         <f>Zeitplanung!AL39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -6143,7 +6107,7 @@
       </c>
       <c r="B32" s="101">
         <f>Zeitplanung!AM39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -6153,16 +6117,16 @@
       </c>
       <c r="B33" s="101">
         <f>Zeitplanung!AN39</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="120" t="s">
+      <c r="A36" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="121"/>
+      <c r="B36" s="206"/>
       <c r="C36" s="3" t="s">
         <v>23</v>
       </c>
@@ -6171,24 +6135,24 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="117" t="s">
+      <c r="A37" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="118"/>
+      <c r="B37" s="203"/>
       <c r="C37" s="101">
         <f>Zeitplanung!C5</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D37" s="101">
         <f>Zeitplanung!D5</f>
-        <v>13.2</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="122" t="s">
+      <c r="A38" s="207" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="123"/>
+      <c r="B38" s="208"/>
       <c r="C38" s="101">
         <f>Zeitplanung!C11</f>
         <v>6</v>
@@ -6199,24 +6163,24 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="117" t="s">
+      <c r="A39" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="118"/>
+      <c r="B39" s="203"/>
       <c r="C39" s="101">
         <f>Zeitplanung!C16</f>
         <v>63.400000000000006</v>
       </c>
       <c r="D39" s="101">
         <f>Zeitplanung!D16</f>
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="122" t="s">
+      <c r="A40" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="123"/>
+      <c r="B40" s="208"/>
       <c r="C40" s="101">
         <f>Zeitplanung!C29</f>
         <v>6</v>
@@ -6227,10 +6191,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="117" t="s">
+      <c r="A41" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="118"/>
+      <c r="B41" s="203"/>
       <c r="C41" s="101">
         <f>Zeitplanung!C33</f>
         <v>5</v>
@@ -6241,10 +6205,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="117" t="s">
+      <c r="A42" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="118"/>
+      <c r="B42" s="203"/>
       <c r="C42" s="101">
         <f>Zeitplanung!C36</f>
         <v>0</v>

</xml_diff>

<commit_message>
Updated Project Errors in Mail service
</commit_message>
<xml_diff>
--- a/Documents/Zeitplanung.xlsx
+++ b/Documents/Zeitplanung.xlsx
@@ -2143,6 +2143,18 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="63" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2187,18 +2199,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="80" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="63" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Akzent3" xfId="1" builtinId="37"/>
@@ -2437,10 +2437,10 @@
                   <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2479,7 +2479,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2505,11 +2505,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="309416064"/>
-        <c:axId val="309419984"/>
+        <c:axId val="316088096"/>
+        <c:axId val="316088488"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="309416064"/>
+        <c:axId val="316088096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2519,14 +2519,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309419984"/>
+        <c:crossAx val="316088488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="309419984"/>
+        <c:axId val="316088488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2537,7 +2537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309416064"/>
+        <c:crossAx val="316088096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2707,7 +2707,7 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.900000000000002</c:v>
+                  <c:v>46.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2736,11 +2736,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="309416848"/>
-        <c:axId val="309421944"/>
+        <c:axId val="316084568"/>
+        <c:axId val="316089272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="309416848"/>
+        <c:axId val="316084568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,7 +2750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309421944"/>
+        <c:crossAx val="316089272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2758,7 +2758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309421944"/>
+        <c:axId val="316089272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2769,7 +2769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309416848"/>
+        <c:crossAx val="316084568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3210,8 +3210,8 @@
   </sheetPr>
   <dimension ref="A1:AS44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="AM17" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3234,38 +3234,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="197" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="193"/>
-      <c r="L1" s="193"/>
-      <c r="M1" s="193"/>
-      <c r="N1" s="193"/>
-      <c r="O1" s="193"/>
-      <c r="P1" s="193"/>
-      <c r="Q1" s="193"/>
-      <c r="R1" s="193"/>
-      <c r="S1" s="193"/>
-      <c r="T1" s="193"/>
-      <c r="U1" s="193"/>
-      <c r="V1" s="193"/>
-      <c r="W1" s="193"/>
-      <c r="X1" s="193"/>
-      <c r="Y1" s="193"/>
-      <c r="Z1" s="193"/>
-      <c r="AA1" s="193"/>
-      <c r="AB1" s="193"/>
-      <c r="AC1" s="193"/>
-      <c r="AD1" s="193"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
+      <c r="F1" s="197"/>
+      <c r="G1" s="197"/>
+      <c r="H1" s="197"/>
+      <c r="I1" s="197"/>
+      <c r="J1" s="197"/>
+      <c r="K1" s="197"/>
+      <c r="L1" s="197"/>
+      <c r="M1" s="197"/>
+      <c r="N1" s="197"/>
+      <c r="O1" s="197"/>
+      <c r="P1" s="197"/>
+      <c r="Q1" s="197"/>
+      <c r="R1" s="197"/>
+      <c r="S1" s="197"/>
+      <c r="T1" s="197"/>
+      <c r="U1" s="197"/>
+      <c r="V1" s="197"/>
+      <c r="W1" s="197"/>
+      <c r="X1" s="197"/>
+      <c r="Y1" s="197"/>
+      <c r="Z1" s="197"/>
+      <c r="AA1" s="197"/>
+      <c r="AB1" s="197"/>
+      <c r="AC1" s="197"/>
+      <c r="AD1" s="197"/>
     </row>
     <row r="2" spans="1:45" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
@@ -3284,65 +3284,65 @@
     <row r="3" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="52"/>
       <c r="B3" s="56"/>
-      <c r="C3" s="195" t="s">
+      <c r="C3" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="195"/>
+      <c r="D3" s="199"/>
       <c r="E3" s="16"/>
       <c r="F3" s="17"/>
       <c r="G3" s="19"/>
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="195" t="s">
+      <c r="K3" s="199" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="196"/>
-      <c r="P3" s="194" t="s">
+      <c r="L3" s="199"/>
+      <c r="M3" s="199"/>
+      <c r="N3" s="199"/>
+      <c r="O3" s="200"/>
+      <c r="P3" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="195"/>
-      <c r="S3" s="195"/>
-      <c r="T3" s="195"/>
-      <c r="U3" s="194" t="s">
+      <c r="Q3" s="199"/>
+      <c r="R3" s="199"/>
+      <c r="S3" s="199"/>
+      <c r="T3" s="199"/>
+      <c r="U3" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="195"/>
-      <c r="W3" s="195"/>
-      <c r="X3" s="195"/>
-      <c r="Y3" s="195"/>
-      <c r="Z3" s="194" t="s">
+      <c r="V3" s="199"/>
+      <c r="W3" s="199"/>
+      <c r="X3" s="199"/>
+      <c r="Y3" s="199"/>
+      <c r="Z3" s="198" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="195"/>
-      <c r="AB3" s="195"/>
-      <c r="AC3" s="195"/>
-      <c r="AD3" s="195"/>
-      <c r="AE3" s="194" t="s">
+      <c r="AA3" s="199"/>
+      <c r="AB3" s="199"/>
+      <c r="AC3" s="199"/>
+      <c r="AD3" s="199"/>
+      <c r="AE3" s="198" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" s="195"/>
-      <c r="AG3" s="195"/>
-      <c r="AH3" s="195"/>
-      <c r="AI3" s="195"/>
-      <c r="AJ3" s="194" t="s">
+      <c r="AF3" s="199"/>
+      <c r="AG3" s="199"/>
+      <c r="AH3" s="199"/>
+      <c r="AI3" s="199"/>
+      <c r="AJ3" s="198" t="s">
         <v>35</v>
       </c>
-      <c r="AK3" s="195"/>
-      <c r="AL3" s="195"/>
-      <c r="AM3" s="195"/>
-      <c r="AN3" s="197"/>
-      <c r="AO3" s="194" t="s">
+      <c r="AK3" s="199"/>
+      <c r="AL3" s="199"/>
+      <c r="AM3" s="199"/>
+      <c r="AN3" s="201"/>
+      <c r="AO3" s="198" t="s">
         <v>35</v>
       </c>
-      <c r="AP3" s="195"/>
-      <c r="AQ3" s="195"/>
-      <c r="AR3" s="195"/>
-      <c r="AS3" s="197"/>
+      <c r="AP3" s="199"/>
+      <c r="AQ3" s="199"/>
+      <c r="AR3" s="199"/>
+      <c r="AS3" s="201"/>
     </row>
     <row r="4" spans="1:45" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="87" t="s">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="D16" s="76">
         <f>SUM(D17:D23)</f>
-        <v>22.900000000000002</v>
+        <v>46.400000000000006</v>
       </c>
       <c r="E16" s="77"/>
       <c r="F16" s="78"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="D17" s="45">
         <f t="shared" ref="D17:D22" si="1">IF(SUM(K17:AS17)=0," ",SUM(K17:AS17))</f>
-        <v>18.400000000000002</v>
+        <v>22.400000000000002</v>
       </c>
       <c r="E17" s="31">
         <v>1</v>
@@ -4252,7 +4252,9 @@
       <c r="AI17" s="117"/>
       <c r="AJ17" s="118"/>
       <c r="AK17" s="112"/>
-      <c r="AL17" s="113"/>
+      <c r="AL17" s="189">
+        <v>4</v>
+      </c>
       <c r="AM17" s="156"/>
       <c r="AN17" s="157"/>
       <c r="AO17" s="118"/>
@@ -4271,9 +4273,9 @@
       <c r="C18" s="32">
         <v>4.5</v>
       </c>
-      <c r="D18" s="45" t="str">
+      <c r="D18" s="45">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>4.5</v>
       </c>
       <c r="E18" s="31">
         <v>1</v>
@@ -4310,7 +4312,9 @@
       <c r="AI18" s="117"/>
       <c r="AJ18" s="118"/>
       <c r="AK18" s="112"/>
-      <c r="AL18" s="113"/>
+      <c r="AL18" s="189">
+        <v>4.5</v>
+      </c>
       <c r="AM18" s="156"/>
       <c r="AN18" s="157"/>
       <c r="AO18" s="118"/>
@@ -4356,7 +4360,7 @@
       <c r="U19" s="118"/>
       <c r="V19" s="112"/>
       <c r="W19" s="108"/>
-      <c r="X19" s="180"/>
+      <c r="X19" s="113"/>
       <c r="Y19" s="185"/>
       <c r="Z19" s="159"/>
       <c r="AA19" s="116"/>
@@ -4391,7 +4395,7 @@
       </c>
       <c r="D20" s="156">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>19.5</v>
       </c>
       <c r="E20" s="31">
         <v>1</v>
@@ -4416,8 +4420,12 @@
       <c r="W20" s="177">
         <v>4.5</v>
       </c>
-      <c r="X20" s="113"/>
-      <c r="Y20" s="114"/>
+      <c r="X20" s="189">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="191">
+        <v>7</v>
+      </c>
       <c r="Z20" s="159"/>
       <c r="AA20" s="116"/>
       <c r="AB20" s="109"/>
@@ -5484,7 +5492,7 @@
       </c>
       <c r="D39" s="90">
         <f>SUM(D36+D33+D29+D16+D11+D5)</f>
-        <v>38</v>
+        <v>61.500000000000007</v>
       </c>
       <c r="E39" s="90"/>
       <c r="F39" s="90"/>
@@ -5492,158 +5500,158 @@
       <c r="H39" s="90"/>
       <c r="I39" s="91"/>
       <c r="J39" s="92"/>
-      <c r="K39" s="209">
+      <c r="K39" s="193">
         <f t="shared" ref="K39:AS39" si="2">SUM(K5:K38)</f>
         <v>0</v>
       </c>
-      <c r="L39" s="210">
+      <c r="L39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M39" s="208">
+      <c r="M39" s="192">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N39" s="208">
+      <c r="N39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O39" s="208">
+      <c r="O39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P39" s="208">
+      <c r="P39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q39" s="210">
+      <c r="Q39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R39" s="208">
+      <c r="R39" s="192">
         <f t="shared" si="2"/>
         <v>6.9</v>
       </c>
-      <c r="S39" s="210">
+      <c r="S39" s="194">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="T39" s="208">
+      <c r="T39" s="192">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="U39" s="208">
+      <c r="U39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V39" s="210">
+      <c r="V39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W39" s="208">
+      <c r="W39" s="192">
         <f t="shared" si="2"/>
         <v>7.6</v>
       </c>
-      <c r="X39" s="210">
+      <c r="X39" s="194">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Y39" s="192">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="Z39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y39" s="208">
+      <c r="AA39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z39" s="208">
+      <c r="AB39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA39" s="210">
+      <c r="AC39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB39" s="208">
+      <c r="AD39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC39" s="210">
+      <c r="AE39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD39" s="208">
+      <c r="AF39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE39" s="208">
+      <c r="AG39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF39" s="210">
+      <c r="AH39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG39" s="208">
+      <c r="AI39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH39" s="210">
+      <c r="AJ39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI39" s="208">
+      <c r="AK39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AJ39" s="208">
+      <c r="AL39" s="192">
+        <f t="shared" si="2"/>
+        <v>8.5</v>
+      </c>
+      <c r="AM39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AK39" s="210">
+      <c r="AN39" s="195">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AL39" s="208">
+      <c r="AO39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AM39" s="210">
+      <c r="AP39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AN39" s="211">
+      <c r="AQ39" s="192">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO39" s="208">
+      <c r="AR39" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AP39" s="210">
+      <c r="AS39" s="195">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AQ39" s="208">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AR39" s="210">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AS39" s="211">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="93"/>
-      <c r="B40" s="192"/>
-      <c r="C40" s="192"/>
-      <c r="D40" s="192"/>
-      <c r="E40" s="192"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="192"/>
-      <c r="H40" s="192"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
+      <c r="B40" s="196"/>
+      <c r="C40" s="196"/>
+      <c r="D40" s="196"/>
+      <c r="E40" s="196"/>
+      <c r="F40" s="196"/>
+      <c r="G40" s="196"/>
+      <c r="H40" s="196"/>
+      <c r="I40" s="196"/>
+      <c r="J40" s="196"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="104"/>
@@ -5658,26 +5666,26 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
-      <c r="K41" s="199"/>
-      <c r="L41" s="200"/>
-      <c r="M41" s="200"/>
-      <c r="N41" s="200"/>
-      <c r="O41" s="200"/>
-      <c r="P41" s="200"/>
-      <c r="Q41" s="200"/>
-      <c r="R41" s="200"/>
-      <c r="S41" s="200"/>
-      <c r="T41" s="200"/>
-      <c r="U41" s="200"/>
-      <c r="V41" s="200"/>
-      <c r="W41" s="200"/>
-      <c r="X41" s="200"/>
-      <c r="Y41" s="200"/>
-      <c r="Z41" s="200"/>
-      <c r="AA41" s="200"/>
-      <c r="AB41" s="200"/>
-      <c r="AC41" s="200"/>
-      <c r="AD41" s="200"/>
+      <c r="K41" s="203"/>
+      <c r="L41" s="204"/>
+      <c r="M41" s="204"/>
+      <c r="N41" s="204"/>
+      <c r="O41" s="204"/>
+      <c r="P41" s="204"/>
+      <c r="Q41" s="204"/>
+      <c r="R41" s="204"/>
+      <c r="S41" s="204"/>
+      <c r="T41" s="204"/>
+      <c r="U41" s="204"/>
+      <c r="V41" s="204"/>
+      <c r="W41" s="204"/>
+      <c r="X41" s="204"/>
+      <c r="Y41" s="204"/>
+      <c r="Z41" s="204"/>
+      <c r="AA41" s="204"/>
+      <c r="AB41" s="204"/>
+      <c r="AC41" s="204"/>
+      <c r="AD41" s="204"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="103"/>
@@ -5692,26 +5700,26 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
-      <c r="K42" s="198"/>
-      <c r="L42" s="198"/>
-      <c r="M42" s="198"/>
-      <c r="N42" s="198"/>
-      <c r="O42" s="198"/>
-      <c r="P42" s="198"/>
-      <c r="Q42" s="198"/>
-      <c r="R42" s="198"/>
-      <c r="S42" s="198"/>
-      <c r="T42" s="198"/>
-      <c r="U42" s="198"/>
-      <c r="V42" s="198"/>
-      <c r="W42" s="198"/>
-      <c r="X42" s="198"/>
-      <c r="Y42" s="198"/>
-      <c r="Z42" s="198"/>
-      <c r="AA42" s="198"/>
-      <c r="AB42" s="198"/>
-      <c r="AC42" s="198"/>
-      <c r="AD42" s="198"/>
+      <c r="K42" s="202"/>
+      <c r="L42" s="202"/>
+      <c r="M42" s="202"/>
+      <c r="N42" s="202"/>
+      <c r="O42" s="202"/>
+      <c r="P42" s="202"/>
+      <c r="Q42" s="202"/>
+      <c r="R42" s="202"/>
+      <c r="S42" s="202"/>
+      <c r="T42" s="202"/>
+      <c r="U42" s="202"/>
+      <c r="V42" s="202"/>
+      <c r="W42" s="202"/>
+      <c r="X42" s="202"/>
+      <c r="Y42" s="202"/>
+      <c r="Z42" s="202"/>
+      <c r="AA42" s="202"/>
+      <c r="AB42" s="202"/>
+      <c r="AC42" s="202"/>
+      <c r="AD42" s="202"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="105"/>
@@ -5726,26 +5734,26 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
-      <c r="K43" s="198"/>
-      <c r="L43" s="198"/>
-      <c r="M43" s="198"/>
-      <c r="N43" s="198"/>
-      <c r="O43" s="198"/>
-      <c r="P43" s="198"/>
-      <c r="Q43" s="198"/>
-      <c r="R43" s="198"/>
-      <c r="S43" s="198"/>
-      <c r="T43" s="198"/>
-      <c r="U43" s="198"/>
-      <c r="V43" s="198"/>
-      <c r="W43" s="198"/>
-      <c r="X43" s="198"/>
-      <c r="Y43" s="198"/>
-      <c r="Z43" s="198"/>
-      <c r="AA43" s="198"/>
-      <c r="AB43" s="198"/>
-      <c r="AC43" s="198"/>
-      <c r="AD43" s="198"/>
+      <c r="K43" s="202"/>
+      <c r="L43" s="202"/>
+      <c r="M43" s="202"/>
+      <c r="N43" s="202"/>
+      <c r="O43" s="202"/>
+      <c r="P43" s="202"/>
+      <c r="Q43" s="202"/>
+      <c r="R43" s="202"/>
+      <c r="S43" s="202"/>
+      <c r="T43" s="202"/>
+      <c r="U43" s="202"/>
+      <c r="V43" s="202"/>
+      <c r="W43" s="202"/>
+      <c r="X43" s="202"/>
+      <c r="Y43" s="202"/>
+      <c r="Z43" s="202"/>
+      <c r="AA43" s="202"/>
+      <c r="AB43" s="202"/>
+      <c r="AC43" s="202"/>
+      <c r="AD43" s="202"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="179"/>
@@ -5800,20 +5808,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="203"/>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
-      <c r="M1" s="203"/>
-      <c r="N1" s="203"/>
+      <c r="A1" s="207"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="207"/>
+      <c r="I1" s="207"/>
+      <c r="J1" s="207"/>
+      <c r="K1" s="207"/>
+      <c r="L1" s="207"/>
+      <c r="M1" s="207"/>
+      <c r="N1" s="207"/>
     </row>
     <row r="2" spans="1:14" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="97"/>
@@ -5976,7 +5984,7 @@
       </c>
       <c r="B17" s="98">
         <f>Zeitplanung!X39</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5986,7 +5994,7 @@
       </c>
       <c r="B18" s="98">
         <f>Zeitplanung!Y39</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -6116,7 +6124,7 @@
       </c>
       <c r="B31" s="98">
         <f>Zeitplanung!AL39</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -6142,10 +6150,10 @@
     <row r="34" spans="1:4" ht="15.5" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="204" t="s">
+      <c r="A36" s="208" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="205"/>
+      <c r="B36" s="209"/>
       <c r="C36" s="3" t="s">
         <v>23</v>
       </c>
@@ -6154,10 +6162,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="201" t="s">
+      <c r="A37" s="205" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="202"/>
+      <c r="B37" s="206"/>
       <c r="C37" s="98">
         <f>Zeitplanung!C5</f>
         <v>22</v>
@@ -6168,10 +6176,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="206" t="s">
+      <c r="A38" s="210" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="207"/>
+      <c r="B38" s="211"/>
       <c r="C38" s="98">
         <f>Zeitplanung!C11</f>
         <v>6</v>
@@ -6182,24 +6190,24 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="201" t="s">
+      <c r="A39" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="202"/>
+      <c r="B39" s="206"/>
       <c r="C39" s="98">
         <f>Zeitplanung!C16</f>
         <v>63.400000000000006</v>
       </c>
       <c r="D39" s="98">
         <f>Zeitplanung!D16</f>
-        <v>22.900000000000002</v>
+        <v>46.400000000000006</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="206" t="s">
+      <c r="A40" s="210" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="207"/>
+      <c r="B40" s="211"/>
       <c r="C40" s="98">
         <f>Zeitplanung!C29</f>
         <v>6</v>
@@ -6210,10 +6218,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="201" t="s">
+      <c r="A41" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="202"/>
+      <c r="B41" s="206"/>
       <c r="C41" s="98">
         <f>Zeitplanung!C33</f>
         <v>5</v>
@@ -6224,10 +6232,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="201" t="s">
+      <c r="A42" s="205" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="202"/>
+      <c r="B42" s="206"/>
       <c r="C42" s="98">
         <f>Zeitplanung!C36</f>
         <v>0</v>

</xml_diff>